<commit_message>
amélioration de la doc et ajout du scripte de schéme de DB
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -772,6 +772,12 @@
     <xf numFmtId="0" fontId="30" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,6 +812,12 @@
     <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -815,12 +827,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -835,12 +841,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="25" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1184,17 +1184,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
       <c r="K2" s="9"/>
       <c r="L2" s="50"/>
       <c r="M2" s="53"/>
@@ -1254,77 +1254,77 @@
     </row>
     <row r="4" spans="1:41" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="71" t="s">
+      <c r="C4" s="72"/>
+      <c r="D4" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="15"/>
-      <c r="L4" s="69" t="s">
+      <c r="L4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="72" t="s">
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
+      <c r="V4" s="72"/>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
     </row>
     <row r="5" spans="1:41" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="79" t="s">
+      <c r="C5" s="72"/>
+      <c r="D5" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="15"/>
-      <c r="L5" s="69" t="s">
+      <c r="L5" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="80">
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="72"/>
+      <c r="U5" s="77">
         <v>44319</v>
       </c>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="72"/>
+      <c r="Y5" s="72"/>
+      <c r="Z5" s="72"/>
+      <c r="AA5" s="72"/>
     </row>
     <row r="6" spans="1:41" ht="21" customHeight="1">
       <c r="A6" s="17"/>
@@ -1388,187 +1388,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="76" t="s">
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="77"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="77"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="62" t="s">
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="81"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="63"/>
-      <c r="AA8" s="63"/>
-      <c r="AB8" s="63"/>
-      <c r="AC8" s="63"/>
-      <c r="AD8" s="63"/>
-      <c r="AE8" s="63"/>
-      <c r="AF8" s="63"/>
-      <c r="AG8" s="63"/>
-      <c r="AH8" s="63"/>
-      <c r="AL8" s="60"/>
-      <c r="AM8" s="61"/>
-      <c r="AN8" s="61"/>
-      <c r="AO8" s="61"/>
+      <c r="Z8" s="65"/>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="65"/>
+      <c r="AE8" s="65"/>
+      <c r="AF8" s="65"/>
+      <c r="AG8" s="65"/>
+      <c r="AH8" s="65"/>
+      <c r="AL8" s="62"/>
+      <c r="AM8" s="63"/>
+      <c r="AN8" s="63"/>
+      <c r="AO8" s="63"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="66" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="65"/>
-      <c r="G9" s="66" t="s">
+      <c r="F9" s="67"/>
+      <c r="G9" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="65"/>
-      <c r="I9" s="66" t="s">
+      <c r="H9" s="67"/>
+      <c r="I9" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="65"/>
-      <c r="K9" s="66" t="s">
+      <c r="J9" s="67"/>
+      <c r="K9" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="65"/>
-      <c r="M9" s="66" t="s">
+      <c r="L9" s="67"/>
+      <c r="M9" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="65"/>
-      <c r="O9" s="73" t="s">
+      <c r="N9" s="67"/>
+      <c r="O9" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="73" t="s">
+      <c r="P9" s="67"/>
+      <c r="Q9" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="65"/>
-      <c r="S9" s="73" t="s">
+      <c r="R9" s="67"/>
+      <c r="S9" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="65"/>
-      <c r="U9" s="73" t="s">
+      <c r="T9" s="67"/>
+      <c r="U9" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="65"/>
-      <c r="W9" s="73" t="s">
+      <c r="V9" s="67"/>
+      <c r="W9" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="65"/>
-      <c r="Y9" s="66" t="s">
+      <c r="X9" s="67"/>
+      <c r="Y9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="66" t="s">
+      <c r="Z9" s="67"/>
+      <c r="AA9" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="64" t="s">
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="65"/>
-      <c r="AE9" s="64" t="s">
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="64" t="s">
+      <c r="AF9" s="67"/>
+      <c r="AG9" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="65"/>
+      <c r="AH9" s="67"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="66" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="65"/>
-      <c r="G10" s="66" t="s">
+      <c r="F10" s="67"/>
+      <c r="G10" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="65"/>
-      <c r="I10" s="66" t="s">
+      <c r="H10" s="67"/>
+      <c r="I10" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="65"/>
-      <c r="K10" s="66" t="s">
+      <c r="J10" s="67"/>
+      <c r="K10" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="65"/>
-      <c r="M10" s="66" t="s">
+      <c r="L10" s="67"/>
+      <c r="M10" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="65"/>
-      <c r="O10" s="73" t="s">
+      <c r="N10" s="67"/>
+      <c r="O10" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="73" t="s">
+      <c r="P10" s="67"/>
+      <c r="Q10" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="65"/>
-      <c r="S10" s="73" t="s">
+      <c r="R10" s="67"/>
+      <c r="S10" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="65"/>
-      <c r="U10" s="73" t="s">
+      <c r="T10" s="67"/>
+      <c r="U10" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="65"/>
-      <c r="W10" s="73" t="s">
+      <c r="V10" s="67"/>
+      <c r="W10" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="65"/>
-      <c r="Y10" s="66" t="s">
+      <c r="X10" s="67"/>
+      <c r="Y10" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="65"/>
-      <c r="AA10" s="66" t="s">
+      <c r="Z10" s="67"/>
+      <c r="AA10" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="65"/>
-      <c r="AC10" s="66" t="s">
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="65"/>
-      <c r="AE10" s="66" t="s">
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="65"/>
-      <c r="AG10" s="66" t="s">
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="65"/>
+      <c r="AH10" s="67"/>
       <c r="AI10" s="51" t="s">
         <v>24</v>
       </c>
@@ -1622,11 +1622,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="83" t="s">
+      <c r="B12" s="83"/>
+      <c r="C12" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="84">
+      <c r="D12" s="86">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1662,10 +1662,10 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="87"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="60"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
@@ -1698,11 +1698,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="85"/>
-      <c r="C14" s="83" t="s">
+      <c r="B14" s="87"/>
+      <c r="C14" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="84">
+      <c r="D14" s="86">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1738,10 +1738,10 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="87"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
@@ -1774,11 +1774,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="83" t="s">
+      <c r="B16" s="83"/>
+      <c r="C16" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="84">
+      <c r="D16" s="86">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1814,10 +1814,10 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="87"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
@@ -1850,11 +1850,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="83" t="s">
+      <c r="B18" s="83"/>
+      <c r="C18" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="84">
+      <c r="D18" s="86">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1890,11 +1890,11 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
       <c r="E19" s="37"/>
-      <c r="F19" s="87"/>
+      <c r="F19" s="60"/>
       <c r="G19" s="36"/>
       <c r="H19" s="36"/>
       <c r="I19" s="37"/>
@@ -1926,11 +1926,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="83" t="s">
+      <c r="B20" s="83"/>
+      <c r="C20" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="84">
+      <c r="D20" s="86">
         <v>1</v>
       </c>
       <c r="E20" s="58"/>
@@ -1966,10 +1966,10 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="88"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="61"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
       <c r="H21" s="36"/>
@@ -2002,11 +2002,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="83" t="s">
+      <c r="B22" s="83"/>
+      <c r="C22" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="84">
+      <c r="D22" s="86">
         <v>2</v>
       </c>
       <c r="E22" s="54"/>
@@ -2042,11 +2042,11 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="82"/>
-      <c r="D23" s="82"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="36"/>
-      <c r="F23" s="37"/>
+      <c r="F23" s="60"/>
       <c r="G23" s="36"/>
       <c r="H23" s="36"/>
       <c r="I23" s="37"/>
@@ -2125,11 +2125,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="83" t="s">
+      <c r="B25" s="83"/>
+      <c r="C25" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="84">
+      <c r="D25" s="86">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2165,9 +2165,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="82"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="37"/>
@@ -2201,11 +2201,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="83" t="s">
+      <c r="B27" s="83"/>
+      <c r="C27" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="84">
+      <c r="D27" s="86">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2241,9 +2241,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="82"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2277,11 +2277,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="83" t="s">
+      <c r="B29" s="83"/>
+      <c r="C29" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="84">
+      <c r="D29" s="86">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2317,9 +2317,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="82"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2353,11 +2353,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="83" t="s">
+      <c r="B31" s="83"/>
+      <c r="C31" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="84">
+      <c r="D31" s="86">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2393,9 +2393,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="82"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2429,11 +2429,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="81"/>
-      <c r="C33" s="83" t="s">
+      <c r="B33" s="83"/>
+      <c r="C33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="84">
+      <c r="D33" s="86">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2468,9 +2468,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="82"/>
-      <c r="C34" s="82"/>
-      <c r="D34" s="82"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2504,11 +2504,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="81"/>
-      <c r="C35" s="83" t="s">
+      <c r="B35" s="83"/>
+      <c r="C35" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="84">
+      <c r="D35" s="86">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2543,9 +2543,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="82"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="82"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
@@ -2579,11 +2579,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="81"/>
-      <c r="C37" s="83" t="s">
+      <c r="B37" s="83"/>
+      <c r="C37" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="84">
+      <c r="D37" s="86">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2618,9 +2618,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="82"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="84"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2654,11 +2654,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="81"/>
-      <c r="C39" s="83" t="s">
+      <c r="B39" s="83"/>
+      <c r="C39" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="84">
+      <c r="D39" s="86">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2693,9 +2693,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="82"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2729,11 +2729,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="81"/>
-      <c r="C41" s="83" t="s">
+      <c r="B41" s="83"/>
+      <c r="C41" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="84">
+      <c r="D41" s="86">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2769,9 +2769,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="82"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="82"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2852,11 +2852,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="81"/>
-      <c r="C44" s="83" t="s">
+      <c r="B44" s="83"/>
+      <c r="C44" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="84">
+      <c r="D44" s="86">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2892,9 +2892,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
       <c r="E45" s="48"/>
       <c r="F45" s="46"/>
       <c r="G45" s="46"/>
@@ -2928,11 +2928,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="81"/>
-      <c r="C46" s="83" t="s">
+      <c r="B46" s="83"/>
+      <c r="C46" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="84">
+      <c r="D46" s="86">
         <v>24</v>
       </c>
       <c r="E46" s="48"/>
@@ -2968,11 +2968,11 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="46"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="61"/>
       <c r="G47" s="46"/>
       <c r="H47" s="39"/>
       <c r="I47" s="39"/>
@@ -3004,11 +3004,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="81"/>
-      <c r="C48" s="83" t="s">
+      <c r="B48" s="83"/>
+      <c r="C48" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="84">
+      <c r="D48" s="86">
         <v>5</v>
       </c>
       <c r="E48" s="47"/>
@@ -3044,11 +3044,11 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="82"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
       <c r="G49" s="39"/>
       <c r="H49" s="39"/>
       <c r="I49" s="39"/>
@@ -3086,16 +3086,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="86"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="86"/>
-      <c r="H50" s="75"/>
-      <c r="I50" s="86"/>
-      <c r="J50" s="75"/>
-      <c r="K50" s="86"/>
-      <c r="L50" s="75"/>
-      <c r="M50" s="86"/>
-      <c r="N50" s="75"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="88"/>
+      <c r="J50" s="79"/>
+      <c r="K50" s="88"/>
+      <c r="L50" s="79"/>
+      <c r="M50" s="88"/>
+      <c r="N50" s="79"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3106,10 +3106,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="86"/>
-      <c r="Z50" s="75"/>
-      <c r="AA50" s="86"/>
-      <c r="AB50" s="75"/>
+      <c r="Y50" s="88"/>
+      <c r="Z50" s="79"/>
+      <c r="AA50" s="88"/>
+      <c r="AB50" s="79"/>
       <c r="AC50" s="51"/>
       <c r="AD50" s="51"/>
       <c r="AE50" s="51"/>

</xml_diff>

<commit_message>
login et register fonctionnel
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -778,55 +778,6 @@
     <xf numFmtId="165" fontId="25" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -837,11 +788,60 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,8 +1135,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1184,17 +1184,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="9"/>
       <c r="L2" s="50"/>
       <c r="M2" s="53"/>
@@ -1258,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="72"/>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="87" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="72"/>
@@ -1279,7 +1279,7 @@
       <c r="R4" s="72"/>
       <c r="S4" s="72"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="88" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="72"/>
@@ -1295,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="72"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="73" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="72"/>
@@ -1316,7 +1316,7 @@
       <c r="R5" s="72"/>
       <c r="S5" s="72"/>
       <c r="T5" s="72"/>
-      <c r="U5" s="77">
+      <c r="U5" s="74">
         <v>44319</v>
       </c>
       <c r="V5" s="72"/>
@@ -1388,187 +1388,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="80" t="s">
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="81"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="81"/>
-      <c r="V8" s="81"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="82"/>
-      <c r="Y8" s="64" t="s">
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="77"/>
+      <c r="T8" s="77"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="78"/>
+      <c r="Y8" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="65"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="65"/>
-      <c r="AD8" s="65"/>
-      <c r="AE8" s="65"/>
-      <c r="AF8" s="65"/>
-      <c r="AG8" s="65"/>
-      <c r="AH8" s="65"/>
-      <c r="AL8" s="62"/>
-      <c r="AM8" s="63"/>
-      <c r="AN8" s="63"/>
-      <c r="AO8" s="63"/>
+      <c r="Z8" s="83"/>
+      <c r="AA8" s="83"/>
+      <c r="AB8" s="83"/>
+      <c r="AC8" s="83"/>
+      <c r="AD8" s="83"/>
+      <c r="AE8" s="83"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="83"/>
+      <c r="AH8" s="83"/>
+      <c r="AL8" s="80"/>
+      <c r="AM8" s="81"/>
+      <c r="AN8" s="81"/>
+      <c r="AO8" s="81"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="68" t="s">
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="68" t="s">
+      <c r="F9" s="70"/>
+      <c r="G9" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68" t="s">
+      <c r="H9" s="70"/>
+      <c r="I9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="67"/>
-      <c r="K9" s="68" t="s">
+      <c r="J9" s="70"/>
+      <c r="K9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="67"/>
-      <c r="M9" s="68" t="s">
+      <c r="L9" s="70"/>
+      <c r="M9" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="67"/>
-      <c r="O9" s="75" t="s">
+      <c r="N9" s="70"/>
+      <c r="O9" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="75" t="s">
+      <c r="P9" s="70"/>
+      <c r="Q9" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="67"/>
-      <c r="S9" s="75" t="s">
+      <c r="R9" s="70"/>
+      <c r="S9" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="67"/>
-      <c r="U9" s="75" t="s">
+      <c r="T9" s="70"/>
+      <c r="U9" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="67"/>
-      <c r="W9" s="75" t="s">
+      <c r="V9" s="70"/>
+      <c r="W9" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="67"/>
-      <c r="Y9" s="68" t="s">
+      <c r="X9" s="70"/>
+      <c r="Y9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="67"/>
-      <c r="AA9" s="68" t="s">
+      <c r="Z9" s="70"/>
+      <c r="AA9" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="66" t="s">
+      <c r="AB9" s="70"/>
+      <c r="AC9" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="67"/>
-      <c r="AE9" s="66" t="s">
+      <c r="AD9" s="70"/>
+      <c r="AE9" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="67"/>
-      <c r="AG9" s="66" t="s">
+      <c r="AF9" s="70"/>
+      <c r="AG9" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="67"/>
+      <c r="AH9" s="70"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="68" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="68" t="s">
+      <c r="F10" s="70"/>
+      <c r="G10" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68" t="s">
+      <c r="H10" s="70"/>
+      <c r="I10" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="67"/>
-      <c r="K10" s="68" t="s">
+      <c r="J10" s="70"/>
+      <c r="K10" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="67"/>
-      <c r="M10" s="68" t="s">
+      <c r="L10" s="70"/>
+      <c r="M10" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="67"/>
-      <c r="O10" s="75" t="s">
+      <c r="N10" s="70"/>
+      <c r="O10" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="75" t="s">
+      <c r="P10" s="70"/>
+      <c r="Q10" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="67"/>
-      <c r="S10" s="75" t="s">
+      <c r="R10" s="70"/>
+      <c r="S10" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="67"/>
-      <c r="U10" s="75" t="s">
+      <c r="T10" s="70"/>
+      <c r="U10" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="67"/>
-      <c r="W10" s="75" t="s">
+      <c r="V10" s="70"/>
+      <c r="W10" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="67"/>
-      <c r="Y10" s="68" t="s">
+      <c r="X10" s="70"/>
+      <c r="Y10" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="68" t="s">
+      <c r="Z10" s="70"/>
+      <c r="AA10" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="68" t="s">
+      <c r="AB10" s="70"/>
+      <c r="AC10" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="68" t="s">
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="67"/>
-      <c r="AG10" s="68" t="s">
+      <c r="AF10" s="70"/>
+      <c r="AG10" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="67"/>
+      <c r="AH10" s="70"/>
       <c r="AI10" s="51" t="s">
         <v>24</v>
       </c>
@@ -1622,11 +1622,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="85" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="65">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1662,9 +1662,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="E13" s="60"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1698,11 +1698,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="85" t="s">
+      <c r="B14" s="68"/>
+      <c r="C14" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="86">
+      <c r="D14" s="65">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1738,9 +1738,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
       <c r="E15" s="60"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1774,11 +1774,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="85" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="86">
+      <c r="D16" s="65">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1814,9 +1814,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="60"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1850,11 +1850,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="85" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="86">
+      <c r="D18" s="65">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1890,9 +1890,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
       <c r="E19" s="37"/>
       <c r="F19" s="60"/>
       <c r="G19" s="36"/>
@@ -1926,11 +1926,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="85" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="86">
+      <c r="D20" s="65">
         <v>1</v>
       </c>
       <c r="E20" s="58"/>
@@ -1966,9 +1966,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
       <c r="E21" s="61"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2002,11 +2002,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="85" t="s">
+      <c r="B22" s="62"/>
+      <c r="C22" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="86">
+      <c r="D22" s="65">
         <v>2</v>
       </c>
       <c r="E22" s="54"/>
@@ -2042,9 +2042,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
       <c r="E23" s="36"/>
       <c r="F23" s="60"/>
       <c r="G23" s="36"/>
@@ -2125,11 +2125,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="85" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="86">
+      <c r="D25" s="65">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2165,12 +2165,12 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
-      <c r="G26" s="37"/>
+      <c r="G26" s="60"/>
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
       <c r="J26" s="37"/>
@@ -2201,11 +2201,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="85" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="86">
+      <c r="D27" s="65">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2241,9 +2241,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2277,11 +2277,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="85" t="s">
+      <c r="B29" s="62"/>
+      <c r="C29" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="86">
+      <c r="D29" s="65">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2317,9 +2317,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2353,11 +2353,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="85" t="s">
+      <c r="B31" s="62"/>
+      <c r="C31" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="86">
+      <c r="D31" s="65">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2393,9 +2393,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2429,11 +2429,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="85" t="s">
+      <c r="B33" s="62"/>
+      <c r="C33" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="86">
+      <c r="D33" s="65">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2468,9 +2468,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2504,11 +2504,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="85" t="s">
+      <c r="B35" s="62"/>
+      <c r="C35" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="86">
+      <c r="D35" s="65">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2543,9 +2543,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="84"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
@@ -2579,11 +2579,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="85" t="s">
+      <c r="B37" s="62"/>
+      <c r="C37" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="86">
+      <c r="D37" s="65">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2618,9 +2618,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
-      <c r="D38" s="84"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2654,11 +2654,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="85" t="s">
+      <c r="B39" s="62"/>
+      <c r="C39" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="86">
+      <c r="D39" s="65">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2693,9 +2693,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="84"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2729,11 +2729,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="83"/>
-      <c r="C41" s="85" t="s">
+      <c r="B41" s="62"/>
+      <c r="C41" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="86">
+      <c r="D41" s="65">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2769,9 +2769,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2852,11 +2852,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="83"/>
-      <c r="C44" s="85" t="s">
+      <c r="B44" s="62"/>
+      <c r="C44" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="86">
+      <c r="D44" s="65">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2892,9 +2892,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="48"/>
       <c r="F45" s="46"/>
       <c r="G45" s="46"/>
@@ -2928,11 +2928,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="83"/>
-      <c r="C46" s="85" t="s">
+      <c r="B46" s="62"/>
+      <c r="C46" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="86">
+      <c r="D46" s="65">
         <v>24</v>
       </c>
       <c r="E46" s="48"/>
@@ -2968,9 +2968,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="84"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="60"/>
       <c r="F47" s="61"/>
       <c r="G47" s="46"/>
@@ -3004,11 +3004,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="83"/>
-      <c r="C48" s="85" t="s">
+      <c r="B48" s="62"/>
+      <c r="C48" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="86">
+      <c r="D48" s="65">
         <v>5</v>
       </c>
       <c r="E48" s="47"/>
@@ -3044,9 +3044,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="84"/>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
       <c r="E49" s="60"/>
       <c r="F49" s="60"/>
       <c r="G49" s="39"/>
@@ -3086,16 +3086,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="88"/>
-      <c r="F50" s="79"/>
-      <c r="G50" s="88"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="88"/>
-      <c r="J50" s="79"/>
-      <c r="K50" s="88"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="88"/>
-      <c r="N50" s="79"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="66"/>
+      <c r="L50" s="67"/>
+      <c r="M50" s="66"/>
+      <c r="N50" s="67"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3106,10 +3106,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="88"/>
-      <c r="Z50" s="79"/>
-      <c r="AA50" s="88"/>
-      <c r="AB50" s="79"/>
+      <c r="Y50" s="66"/>
+      <c r="Z50" s="67"/>
+      <c r="AA50" s="66"/>
+      <c r="AB50" s="67"/>
       <c r="AC50" s="51"/>
       <c r="AD50" s="51"/>
       <c r="AE50" s="51"/>
@@ -3183,43 +3183,52 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="Y8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
@@ -3244,52 +3253,43 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="Y8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
erreur lors de la modification de mot de passe et avancement de la doc
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -778,6 +778,55 @@
     <xf numFmtId="165" fontId="25" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -788,60 +837,11 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1184,17 +1184,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
       <c r="K2" s="9"/>
       <c r="L2" s="50"/>
       <c r="M2" s="53"/>
@@ -1258,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="72"/>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="73" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="72"/>
@@ -1279,7 +1279,7 @@
       <c r="R4" s="72"/>
       <c r="S4" s="72"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="88" t="s">
+      <c r="U4" s="74" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="72"/>
@@ -1295,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="72"/>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="76" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="72"/>
@@ -1316,7 +1316,7 @@
       <c r="R5" s="72"/>
       <c r="S5" s="72"/>
       <c r="T5" s="72"/>
-      <c r="U5" s="74">
+      <c r="U5" s="77">
         <v>44319</v>
       </c>
       <c r="V5" s="72"/>
@@ -1388,187 +1388,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="76" t="s">
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="77"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="77"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="82" t="s">
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="81"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="83"/>
-      <c r="AA8" s="83"/>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83"/>
-      <c r="AE8" s="83"/>
-      <c r="AF8" s="83"/>
-      <c r="AG8" s="83"/>
-      <c r="AH8" s="83"/>
-      <c r="AL8" s="80"/>
-      <c r="AM8" s="81"/>
-      <c r="AN8" s="81"/>
-      <c r="AO8" s="81"/>
+      <c r="Z8" s="65"/>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="65"/>
+      <c r="AE8" s="65"/>
+      <c r="AF8" s="65"/>
+      <c r="AG8" s="65"/>
+      <c r="AH8" s="65"/>
+      <c r="AL8" s="62"/>
+      <c r="AM8" s="63"/>
+      <c r="AN8" s="63"/>
+      <c r="AO8" s="63"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="69" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="69" t="s">
+      <c r="F9" s="67"/>
+      <c r="G9" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="70"/>
-      <c r="I9" s="69" t="s">
+      <c r="H9" s="67"/>
+      <c r="I9" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="70"/>
-      <c r="K9" s="69" t="s">
+      <c r="J9" s="67"/>
+      <c r="K9" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="70"/>
-      <c r="M9" s="69" t="s">
+      <c r="L9" s="67"/>
+      <c r="M9" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="70"/>
-      <c r="O9" s="79" t="s">
+      <c r="N9" s="67"/>
+      <c r="O9" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="79" t="s">
+      <c r="P9" s="67"/>
+      <c r="Q9" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="70"/>
-      <c r="S9" s="79" t="s">
+      <c r="R9" s="67"/>
+      <c r="S9" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="70"/>
-      <c r="U9" s="79" t="s">
+      <c r="T9" s="67"/>
+      <c r="U9" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="70"/>
-      <c r="W9" s="79" t="s">
+      <c r="V9" s="67"/>
+      <c r="W9" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="69" t="s">
+      <c r="X9" s="67"/>
+      <c r="Y9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="69" t="s">
+      <c r="Z9" s="67"/>
+      <c r="AA9" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="70"/>
-      <c r="AC9" s="84" t="s">
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="70"/>
-      <c r="AE9" s="84" t="s">
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="70"/>
-      <c r="AG9" s="84" t="s">
+      <c r="AF9" s="67"/>
+      <c r="AG9" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="70"/>
+      <c r="AH9" s="67"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="69" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="70"/>
-      <c r="G10" s="69" t="s">
+      <c r="F10" s="67"/>
+      <c r="G10" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="70"/>
-      <c r="I10" s="69" t="s">
+      <c r="H10" s="67"/>
+      <c r="I10" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="70"/>
-      <c r="K10" s="69" t="s">
+      <c r="J10" s="67"/>
+      <c r="K10" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="70"/>
-      <c r="M10" s="69" t="s">
+      <c r="L10" s="67"/>
+      <c r="M10" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="70"/>
-      <c r="O10" s="79" t="s">
+      <c r="N10" s="67"/>
+      <c r="O10" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="79" t="s">
+      <c r="P10" s="67"/>
+      <c r="Q10" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="70"/>
-      <c r="S10" s="79" t="s">
+      <c r="R10" s="67"/>
+      <c r="S10" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="70"/>
-      <c r="U10" s="79" t="s">
+      <c r="T10" s="67"/>
+      <c r="U10" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="70"/>
-      <c r="W10" s="79" t="s">
+      <c r="V10" s="67"/>
+      <c r="W10" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="70"/>
-      <c r="Y10" s="69" t="s">
+      <c r="X10" s="67"/>
+      <c r="Y10" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="69" t="s">
+      <c r="Z10" s="67"/>
+      <c r="AA10" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="70"/>
-      <c r="AC10" s="69" t="s">
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="70"/>
-      <c r="AE10" s="69" t="s">
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="70"/>
-      <c r="AG10" s="69" t="s">
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="70"/>
+      <c r="AH10" s="67"/>
       <c r="AI10" s="51" t="s">
         <v>24</v>
       </c>
@@ -1622,11 +1622,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="64" t="s">
+      <c r="B12" s="83"/>
+      <c r="C12" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="86">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1662,9 +1662,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="60"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1698,11 +1698,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="64" t="s">
+      <c r="B14" s="87"/>
+      <c r="C14" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="86">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1738,9 +1738,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
       <c r="E15" s="60"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1774,11 +1774,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="83"/>
+      <c r="C16" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="86">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1814,9 +1814,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="60"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1850,11 +1850,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="64" t="s">
+      <c r="B18" s="83"/>
+      <c r="C18" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="86">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1890,9 +1890,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
       <c r="E19" s="37"/>
       <c r="F19" s="60"/>
       <c r="G19" s="36"/>
@@ -1926,11 +1926,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="83"/>
+      <c r="C20" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="86">
         <v>1</v>
       </c>
       <c r="E20" s="58"/>
@@ -1966,9 +1966,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
       <c r="E21" s="61"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2002,11 +2002,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="83"/>
+      <c r="C22" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="86">
         <v>2</v>
       </c>
       <c r="E22" s="54"/>
@@ -2042,9 +2042,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="36"/>
       <c r="F23" s="60"/>
       <c r="G23" s="36"/>
@@ -2125,11 +2125,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="64" t="s">
+      <c r="B25" s="83"/>
+      <c r="C25" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="86">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2165,9 +2165,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="60"/>
@@ -2201,11 +2201,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="83"/>
+      <c r="C27" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="86">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2241,9 +2241,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2277,11 +2277,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="64" t="s">
+      <c r="B29" s="83"/>
+      <c r="C29" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="86">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2317,9 +2317,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2353,11 +2353,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="64" t="s">
+      <c r="B31" s="83"/>
+      <c r="C31" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="86">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2393,9 +2393,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2429,11 +2429,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="64" t="s">
+      <c r="B33" s="83"/>
+      <c r="C33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="86">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2468,9 +2468,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2504,11 +2504,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="64" t="s">
+      <c r="B35" s="83"/>
+      <c r="C35" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="86">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2543,9 +2543,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
@@ -2579,11 +2579,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="64" t="s">
+      <c r="B37" s="83"/>
+      <c r="C37" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="86">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2618,9 +2618,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="84"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2654,11 +2654,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="64" t="s">
+      <c r="B39" s="83"/>
+      <c r="C39" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="86">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2693,9 +2693,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2729,11 +2729,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="64" t="s">
+      <c r="B41" s="83"/>
+      <c r="C41" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="86">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2769,9 +2769,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2852,11 +2852,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="64" t="s">
+      <c r="B44" s="83"/>
+      <c r="C44" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="86">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2892,9 +2892,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
       <c r="E45" s="48"/>
       <c r="F45" s="46"/>
       <c r="G45" s="46"/>
@@ -2928,11 +2928,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="64" t="s">
+      <c r="B46" s="83"/>
+      <c r="C46" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="86">
         <v>24</v>
       </c>
       <c r="E46" s="48"/>
@@ -2968,12 +2968,12 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
       <c r="E47" s="60"/>
       <c r="F47" s="61"/>
-      <c r="G47" s="46"/>
+      <c r="G47" s="61"/>
       <c r="H47" s="39"/>
       <c r="I47" s="39"/>
       <c r="J47" s="39"/>
@@ -3004,11 +3004,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="64" t="s">
+      <c r="B48" s="83"/>
+      <c r="C48" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="65">
+      <c r="D48" s="86">
         <v>5</v>
       </c>
       <c r="E48" s="47"/>
@@ -3044,12 +3044,12 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
       <c r="E49" s="60"/>
       <c r="F49" s="60"/>
-      <c r="G49" s="39"/>
+      <c r="G49" s="60"/>
       <c r="H49" s="39"/>
       <c r="I49" s="39"/>
       <c r="J49" s="39"/>
@@ -3086,16 +3086,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="66"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="67"/>
-      <c r="K50" s="66"/>
-      <c r="L50" s="67"/>
-      <c r="M50" s="66"/>
-      <c r="N50" s="67"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="88"/>
+      <c r="J50" s="79"/>
+      <c r="K50" s="88"/>
+      <c r="L50" s="79"/>
+      <c r="M50" s="88"/>
+      <c r="N50" s="79"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3106,10 +3106,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="66"/>
-      <c r="Z50" s="67"/>
-      <c r="AA50" s="66"/>
-      <c r="AB50" s="67"/>
+      <c r="Y50" s="88"/>
+      <c r="Z50" s="79"/>
+      <c r="AA50" s="88"/>
+      <c r="AB50" s="79"/>
       <c r="AC50" s="51"/>
       <c r="AD50" s="51"/>
       <c r="AE50" s="51"/>
@@ -3183,6 +3183,89 @@
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="AL8:AO8"/>
     <mergeCell ref="Y8:AH8"/>
     <mergeCell ref="AC9:AD9"/>
@@ -3207,89 +3290,6 @@
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
crud sur les groupes fonctionnel
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -778,55 +778,6 @@
     <xf numFmtId="165" fontId="25" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -837,11 +788,60 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1184,17 +1184,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="9"/>
       <c r="L2" s="50"/>
       <c r="M2" s="53"/>
@@ -1258,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="72"/>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="87" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="72"/>
@@ -1279,7 +1279,7 @@
       <c r="R4" s="72"/>
       <c r="S4" s="72"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="88" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="72"/>
@@ -1295,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="72"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="73" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="72"/>
@@ -1316,7 +1316,7 @@
       <c r="R5" s="72"/>
       <c r="S5" s="72"/>
       <c r="T5" s="72"/>
-      <c r="U5" s="77">
+      <c r="U5" s="74">
         <v>44319</v>
       </c>
       <c r="V5" s="72"/>
@@ -1388,187 +1388,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="80" t="s">
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="81"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="81"/>
-      <c r="V8" s="81"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="82"/>
-      <c r="Y8" s="64" t="s">
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="77"/>
+      <c r="T8" s="77"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="78"/>
+      <c r="Y8" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="65"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="65"/>
-      <c r="AD8" s="65"/>
-      <c r="AE8" s="65"/>
-      <c r="AF8" s="65"/>
-      <c r="AG8" s="65"/>
-      <c r="AH8" s="65"/>
-      <c r="AL8" s="62"/>
-      <c r="AM8" s="63"/>
-      <c r="AN8" s="63"/>
-      <c r="AO8" s="63"/>
+      <c r="Z8" s="83"/>
+      <c r="AA8" s="83"/>
+      <c r="AB8" s="83"/>
+      <c r="AC8" s="83"/>
+      <c r="AD8" s="83"/>
+      <c r="AE8" s="83"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="83"/>
+      <c r="AH8" s="83"/>
+      <c r="AL8" s="80"/>
+      <c r="AM8" s="81"/>
+      <c r="AN8" s="81"/>
+      <c r="AO8" s="81"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="68" t="s">
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="68" t="s">
+      <c r="F9" s="70"/>
+      <c r="G9" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68" t="s">
+      <c r="H9" s="70"/>
+      <c r="I9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="67"/>
-      <c r="K9" s="68" t="s">
+      <c r="J9" s="70"/>
+      <c r="K9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="67"/>
-      <c r="M9" s="68" t="s">
+      <c r="L9" s="70"/>
+      <c r="M9" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="67"/>
-      <c r="O9" s="75" t="s">
+      <c r="N9" s="70"/>
+      <c r="O9" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="75" t="s">
+      <c r="P9" s="70"/>
+      <c r="Q9" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="67"/>
-      <c r="S9" s="75" t="s">
+      <c r="R9" s="70"/>
+      <c r="S9" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="67"/>
-      <c r="U9" s="75" t="s">
+      <c r="T9" s="70"/>
+      <c r="U9" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="67"/>
-      <c r="W9" s="75" t="s">
+      <c r="V9" s="70"/>
+      <c r="W9" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="67"/>
-      <c r="Y9" s="68" t="s">
+      <c r="X9" s="70"/>
+      <c r="Y9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="67"/>
-      <c r="AA9" s="68" t="s">
+      <c r="Z9" s="70"/>
+      <c r="AA9" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="66" t="s">
+      <c r="AB9" s="70"/>
+      <c r="AC9" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="67"/>
-      <c r="AE9" s="66" t="s">
+      <c r="AD9" s="70"/>
+      <c r="AE9" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="67"/>
-      <c r="AG9" s="66" t="s">
+      <c r="AF9" s="70"/>
+      <c r="AG9" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="67"/>
+      <c r="AH9" s="70"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="68" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="68" t="s">
+      <c r="F10" s="70"/>
+      <c r="G10" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68" t="s">
+      <c r="H10" s="70"/>
+      <c r="I10" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="67"/>
-      <c r="K10" s="68" t="s">
+      <c r="J10" s="70"/>
+      <c r="K10" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="67"/>
-      <c r="M10" s="68" t="s">
+      <c r="L10" s="70"/>
+      <c r="M10" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="67"/>
-      <c r="O10" s="75" t="s">
+      <c r="N10" s="70"/>
+      <c r="O10" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="75" t="s">
+      <c r="P10" s="70"/>
+      <c r="Q10" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="67"/>
-      <c r="S10" s="75" t="s">
+      <c r="R10" s="70"/>
+      <c r="S10" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="67"/>
-      <c r="U10" s="75" t="s">
+      <c r="T10" s="70"/>
+      <c r="U10" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="67"/>
-      <c r="W10" s="75" t="s">
+      <c r="V10" s="70"/>
+      <c r="W10" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="67"/>
-      <c r="Y10" s="68" t="s">
+      <c r="X10" s="70"/>
+      <c r="Y10" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="68" t="s">
+      <c r="Z10" s="70"/>
+      <c r="AA10" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="68" t="s">
+      <c r="AB10" s="70"/>
+      <c r="AC10" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="68" t="s">
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="67"/>
-      <c r="AG10" s="68" t="s">
+      <c r="AF10" s="70"/>
+      <c r="AG10" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="67"/>
+      <c r="AH10" s="70"/>
       <c r="AI10" s="51" t="s">
         <v>24</v>
       </c>
@@ -1622,11 +1622,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="85" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="65">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1662,9 +1662,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="E13" s="60"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1698,11 +1698,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="85" t="s">
+      <c r="B14" s="68"/>
+      <c r="C14" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="86">
+      <c r="D14" s="65">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1738,9 +1738,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
       <c r="E15" s="60"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1774,11 +1774,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="85" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="86">
+      <c r="D16" s="65">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1814,9 +1814,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="60"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1850,11 +1850,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="85" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="86">
+      <c r="D18" s="65">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1890,9 +1890,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
       <c r="E19" s="37"/>
       <c r="F19" s="60"/>
       <c r="G19" s="36"/>
@@ -1926,11 +1926,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="85" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="86">
+      <c r="D20" s="65">
         <v>1</v>
       </c>
       <c r="E20" s="58"/>
@@ -1966,9 +1966,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
       <c r="E21" s="61"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2002,11 +2002,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="85" t="s">
+      <c r="B22" s="62"/>
+      <c r="C22" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="86">
+      <c r="D22" s="65">
         <v>2</v>
       </c>
       <c r="E22" s="54"/>
@@ -2042,9 +2042,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
       <c r="E23" s="36"/>
       <c r="F23" s="60"/>
       <c r="G23" s="36"/>
@@ -2125,11 +2125,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="85" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="86">
+      <c r="D25" s="65">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2165,9 +2165,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="60"/>
@@ -2201,11 +2201,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="85" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="86">
+      <c r="D27" s="65">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2241,13 +2241,13 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
+      <c r="H28" s="60"/>
       <c r="I28" s="37"/>
       <c r="J28" s="37"/>
       <c r="K28" s="37"/>
@@ -2277,11 +2277,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="85" t="s">
+      <c r="B29" s="62"/>
+      <c r="C29" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="86">
+      <c r="D29" s="65">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2317,9 +2317,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2353,11 +2353,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="85" t="s">
+      <c r="B31" s="62"/>
+      <c r="C31" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="86">
+      <c r="D31" s="65">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2393,9 +2393,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2429,11 +2429,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="85" t="s">
+      <c r="B33" s="62"/>
+      <c r="C33" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="86">
+      <c r="D33" s="65">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2468,9 +2468,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2504,11 +2504,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="85" t="s">
+      <c r="B35" s="62"/>
+      <c r="C35" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="86">
+      <c r="D35" s="65">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2543,12 +2543,12 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="84"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
+      <c r="G36" s="61"/>
       <c r="H36" s="36"/>
       <c r="I36" s="37"/>
       <c r="J36" s="37"/>
@@ -2579,11 +2579,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="85" t="s">
+      <c r="B37" s="62"/>
+      <c r="C37" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="86">
+      <c r="D37" s="65">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2618,9 +2618,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
-      <c r="D38" s="84"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2654,11 +2654,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="85" t="s">
+      <c r="B39" s="62"/>
+      <c r="C39" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="86">
+      <c r="D39" s="65">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2693,9 +2693,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="84"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2729,11 +2729,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="83"/>
-      <c r="C41" s="85" t="s">
+      <c r="B41" s="62"/>
+      <c r="C41" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="86">
+      <c r="D41" s="65">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2769,9 +2769,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2852,11 +2852,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="83"/>
-      <c r="C44" s="85" t="s">
+      <c r="B44" s="62"/>
+      <c r="C44" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="86">
+      <c r="D44" s="65">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2892,9 +2892,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="48"/>
       <c r="F45" s="46"/>
       <c r="G45" s="46"/>
@@ -2928,11 +2928,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="83"/>
-      <c r="C46" s="85" t="s">
+      <c r="B46" s="62"/>
+      <c r="C46" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="86">
+      <c r="D46" s="65">
         <v>24</v>
       </c>
       <c r="E46" s="48"/>
@@ -2968,13 +2968,13 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="84"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="60"/>
       <c r="F47" s="61"/>
       <c r="G47" s="61"/>
-      <c r="H47" s="39"/>
+      <c r="H47" s="60"/>
       <c r="I47" s="39"/>
       <c r="J47" s="39"/>
       <c r="K47" s="39"/>
@@ -3004,11 +3004,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="83"/>
-      <c r="C48" s="85" t="s">
+      <c r="B48" s="62"/>
+      <c r="C48" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="86">
+      <c r="D48" s="65">
         <v>5</v>
       </c>
       <c r="E48" s="47"/>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="84"/>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
       <c r="E49" s="60"/>
       <c r="F49" s="60"/>
       <c r="G49" s="60"/>
-      <c r="H49" s="39"/>
+      <c r="H49" s="60"/>
       <c r="I49" s="39"/>
       <c r="J49" s="39"/>
       <c r="K49" s="39"/>
@@ -3086,16 +3086,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="88"/>
-      <c r="F50" s="79"/>
-      <c r="G50" s="88"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="88"/>
-      <c r="J50" s="79"/>
-      <c r="K50" s="88"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="88"/>
-      <c r="N50" s="79"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="66"/>
+      <c r="L50" s="67"/>
+      <c r="M50" s="66"/>
+      <c r="N50" s="67"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3106,10 +3106,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="88"/>
-      <c r="Z50" s="79"/>
-      <c r="AA50" s="88"/>
-      <c r="AB50" s="79"/>
+      <c r="Y50" s="66"/>
+      <c r="Z50" s="67"/>
+      <c r="AA50" s="66"/>
+      <c r="AB50" s="67"/>
       <c r="AC50" s="51"/>
       <c r="AD50" s="51"/>
       <c r="AE50" s="51"/>
@@ -3183,43 +3183,52 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="Y8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
@@ -3244,52 +3253,43 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="Y8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Design page principale fini
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -603,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -778,6 +778,55 @@
     <xf numFmtId="165" fontId="25" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -788,61 +837,13 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,8 +1136,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1184,17 +1185,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
       <c r="K2" s="9"/>
       <c r="L2" s="50"/>
       <c r="M2" s="53"/>
@@ -1258,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="72"/>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="73" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="72"/>
@@ -1279,7 +1280,7 @@
       <c r="R4" s="72"/>
       <c r="S4" s="72"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="88" t="s">
+      <c r="U4" s="74" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="72"/>
@@ -1295,7 +1296,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="72"/>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="76" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="72"/>
@@ -1316,7 +1317,7 @@
       <c r="R5" s="72"/>
       <c r="S5" s="72"/>
       <c r="T5" s="72"/>
-      <c r="U5" s="74">
+      <c r="U5" s="77">
         <v>44319</v>
       </c>
       <c r="V5" s="72"/>
@@ -1388,187 +1389,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="76" t="s">
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="77"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="77"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="82" t="s">
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="81"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="83"/>
-      <c r="AA8" s="83"/>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83"/>
-      <c r="AE8" s="83"/>
-      <c r="AF8" s="83"/>
-      <c r="AG8" s="83"/>
-      <c r="AH8" s="83"/>
-      <c r="AL8" s="80"/>
-      <c r="AM8" s="81"/>
-      <c r="AN8" s="81"/>
-      <c r="AO8" s="81"/>
+      <c r="Z8" s="65"/>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="65"/>
+      <c r="AE8" s="65"/>
+      <c r="AF8" s="65"/>
+      <c r="AG8" s="65"/>
+      <c r="AH8" s="65"/>
+      <c r="AL8" s="62"/>
+      <c r="AM8" s="63"/>
+      <c r="AN8" s="63"/>
+      <c r="AO8" s="63"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="69" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="69" t="s">
+      <c r="F9" s="67"/>
+      <c r="G9" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="70"/>
-      <c r="I9" s="69" t="s">
+      <c r="H9" s="67"/>
+      <c r="I9" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="70"/>
-      <c r="K9" s="69" t="s">
+      <c r="J9" s="67"/>
+      <c r="K9" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="70"/>
-      <c r="M9" s="69" t="s">
+      <c r="L9" s="67"/>
+      <c r="M9" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="70"/>
-      <c r="O9" s="79" t="s">
+      <c r="N9" s="67"/>
+      <c r="O9" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="79" t="s">
+      <c r="P9" s="67"/>
+      <c r="Q9" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="70"/>
-      <c r="S9" s="79" t="s">
+      <c r="R9" s="67"/>
+      <c r="S9" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="70"/>
-      <c r="U9" s="79" t="s">
+      <c r="T9" s="67"/>
+      <c r="U9" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="70"/>
-      <c r="W9" s="79" t="s">
+      <c r="V9" s="67"/>
+      <c r="W9" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="69" t="s">
+      <c r="X9" s="67"/>
+      <c r="Y9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="69" t="s">
+      <c r="Z9" s="67"/>
+      <c r="AA9" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="70"/>
-      <c r="AC9" s="84" t="s">
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="70"/>
-      <c r="AE9" s="84" t="s">
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="70"/>
-      <c r="AG9" s="84" t="s">
+      <c r="AF9" s="67"/>
+      <c r="AG9" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="70"/>
+      <c r="AH9" s="67"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="69" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="70"/>
-      <c r="G10" s="69" t="s">
+      <c r="F10" s="67"/>
+      <c r="G10" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="70"/>
-      <c r="I10" s="69" t="s">
+      <c r="H10" s="67"/>
+      <c r="I10" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="70"/>
-      <c r="K10" s="69" t="s">
+      <c r="J10" s="67"/>
+      <c r="K10" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="70"/>
-      <c r="M10" s="69" t="s">
+      <c r="L10" s="67"/>
+      <c r="M10" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="70"/>
-      <c r="O10" s="79" t="s">
+      <c r="N10" s="67"/>
+      <c r="O10" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="79" t="s">
+      <c r="P10" s="67"/>
+      <c r="Q10" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="70"/>
-      <c r="S10" s="79" t="s">
+      <c r="R10" s="67"/>
+      <c r="S10" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="70"/>
-      <c r="U10" s="79" t="s">
+      <c r="T10" s="67"/>
+      <c r="U10" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="70"/>
-      <c r="W10" s="79" t="s">
+      <c r="V10" s="67"/>
+      <c r="W10" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="70"/>
-      <c r="Y10" s="69" t="s">
+      <c r="X10" s="67"/>
+      <c r="Y10" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="69" t="s">
+      <c r="Z10" s="67"/>
+      <c r="AA10" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="70"/>
-      <c r="AC10" s="69" t="s">
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="70"/>
-      <c r="AE10" s="69" t="s">
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="70"/>
-      <c r="AG10" s="69" t="s">
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="70"/>
+      <c r="AH10" s="67"/>
       <c r="AI10" s="51" t="s">
         <v>24</v>
       </c>
@@ -1622,11 +1623,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="64" t="s">
+      <c r="B12" s="83"/>
+      <c r="C12" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="86">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1662,9 +1663,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="60"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1698,11 +1699,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="64" t="s">
+      <c r="B14" s="87"/>
+      <c r="C14" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="86">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1738,9 +1739,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
       <c r="E15" s="60"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1774,11 +1775,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="83"/>
+      <c r="C16" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="86">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1814,9 +1815,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="60"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1850,11 +1851,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="64" t="s">
+      <c r="B18" s="83"/>
+      <c r="C18" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="86">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1890,9 +1891,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
       <c r="E19" s="37"/>
       <c r="F19" s="60"/>
       <c r="G19" s="36"/>
@@ -1926,11 +1927,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="83"/>
+      <c r="C20" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="86">
         <v>1</v>
       </c>
       <c r="E20" s="58"/>
@@ -1966,9 +1967,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
       <c r="E21" s="61"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2002,11 +2003,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="83"/>
+      <c r="C22" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="86">
         <v>2</v>
       </c>
       <c r="E22" s="54"/>
@@ -2042,9 +2043,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="36"/>
       <c r="F23" s="60"/>
       <c r="G23" s="36"/>
@@ -2125,11 +2126,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="64" t="s">
+      <c r="B25" s="83"/>
+      <c r="C25" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="86">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2165,9 +2166,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="60"/>
@@ -2201,11 +2202,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="83"/>
+      <c r="C27" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="86">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2241,14 +2242,14 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
       <c r="H28" s="60"/>
-      <c r="I28" s="37"/>
+      <c r="I28" s="60"/>
       <c r="J28" s="37"/>
       <c r="K28" s="37"/>
       <c r="L28" s="37"/>
@@ -2277,11 +2278,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="64" t="s">
+      <c r="B29" s="83"/>
+      <c r="C29" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="86">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2317,14 +2318,14 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
       <c r="H30" s="36"/>
-      <c r="I30" s="42"/>
+      <c r="I30" s="89"/>
       <c r="J30" s="37"/>
       <c r="K30" s="37"/>
       <c r="L30" s="37"/>
@@ -2353,11 +2354,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="64" t="s">
+      <c r="B31" s="83"/>
+      <c r="C31" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="86">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2393,9 +2394,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2429,11 +2430,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="64" t="s">
+      <c r="B33" s="83"/>
+      <c r="C33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="86">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2468,9 +2469,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2504,11 +2505,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="64" t="s">
+      <c r="B35" s="83"/>
+      <c r="C35" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="86">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2543,9 +2544,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="61"/>
@@ -2579,11 +2580,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="64" t="s">
+      <c r="B37" s="83"/>
+      <c r="C37" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="86">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2618,9 +2619,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="84"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2654,11 +2655,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="64" t="s">
+      <c r="B39" s="83"/>
+      <c r="C39" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="86">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2693,9 +2694,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2729,11 +2730,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="64" t="s">
+      <c r="B41" s="83"/>
+      <c r="C41" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="86">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2769,9 +2770,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2852,11 +2853,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="64" t="s">
+      <c r="B44" s="83"/>
+      <c r="C44" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="86">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2892,9 +2893,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
       <c r="E45" s="48"/>
       <c r="F45" s="46"/>
       <c r="G45" s="46"/>
@@ -2928,11 +2929,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="64" t="s">
+      <c r="B46" s="83"/>
+      <c r="C46" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="86">
         <v>24</v>
       </c>
       <c r="E46" s="48"/>
@@ -2968,14 +2969,14 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
       <c r="E47" s="60"/>
       <c r="F47" s="61"/>
       <c r="G47" s="61"/>
       <c r="H47" s="60"/>
-      <c r="I47" s="39"/>
+      <c r="I47" s="37"/>
       <c r="J47" s="39"/>
       <c r="K47" s="39"/>
       <c r="L47" s="39"/>
@@ -3004,11 +3005,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="64" t="s">
+      <c r="B48" s="83"/>
+      <c r="C48" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="65">
+      <c r="D48" s="86">
         <v>5</v>
       </c>
       <c r="E48" s="47"/>
@@ -3044,14 +3045,14 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
       <c r="E49" s="60"/>
       <c r="F49" s="60"/>
       <c r="G49" s="60"/>
       <c r="H49" s="60"/>
-      <c r="I49" s="39"/>
+      <c r="I49" s="60"/>
       <c r="J49" s="39"/>
       <c r="K49" s="39"/>
       <c r="L49" s="39"/>
@@ -3086,16 +3087,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="66"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="67"/>
-      <c r="K50" s="66"/>
-      <c r="L50" s="67"/>
-      <c r="M50" s="66"/>
-      <c r="N50" s="67"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="88"/>
+      <c r="J50" s="79"/>
+      <c r="K50" s="88"/>
+      <c r="L50" s="79"/>
+      <c r="M50" s="88"/>
+      <c r="N50" s="79"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3106,10 +3107,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="66"/>
-      <c r="Z50" s="67"/>
-      <c r="AA50" s="66"/>
-      <c r="AB50" s="67"/>
+      <c r="Y50" s="88"/>
+      <c r="Z50" s="79"/>
+      <c r="AA50" s="88"/>
+      <c r="AB50" s="79"/>
       <c r="AC50" s="51"/>
       <c r="AD50" s="51"/>
       <c r="AE50" s="51"/>
@@ -3183,6 +3184,89 @@
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="AL8:AO8"/>
     <mergeCell ref="Y8:AH8"/>
     <mergeCell ref="AC9:AD9"/>
@@ -3207,89 +3291,6 @@
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
génération pdf fonctionnelle et amélioration de la documentation
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -778,55 +778,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -837,11 +788,60 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,8 +1135,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1184,17 +1184,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1258,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="72"/>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="87" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="72"/>
@@ -1279,7 +1279,7 @@
       <c r="R4" s="72"/>
       <c r="S4" s="72"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="88" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="72"/>
@@ -1295,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="72"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="73" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="72"/>
@@ -1316,7 +1316,7 @@
       <c r="R5" s="72"/>
       <c r="S5" s="72"/>
       <c r="T5" s="72"/>
-      <c r="U5" s="77">
+      <c r="U5" s="74">
         <v>44319</v>
       </c>
       <c r="V5" s="72"/>
@@ -1388,187 +1388,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="80" t="s">
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="81"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="81"/>
-      <c r="V8" s="81"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="82"/>
-      <c r="Y8" s="64" t="s">
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="77"/>
+      <c r="T8" s="77"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="78"/>
+      <c r="Y8" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="65"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="65"/>
-      <c r="AD8" s="65"/>
-      <c r="AE8" s="65"/>
-      <c r="AF8" s="65"/>
-      <c r="AG8" s="65"/>
-      <c r="AH8" s="65"/>
-      <c r="AL8" s="62"/>
-      <c r="AM8" s="63"/>
-      <c r="AN8" s="63"/>
-      <c r="AO8" s="63"/>
+      <c r="Z8" s="83"/>
+      <c r="AA8" s="83"/>
+      <c r="AB8" s="83"/>
+      <c r="AC8" s="83"/>
+      <c r="AD8" s="83"/>
+      <c r="AE8" s="83"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="83"/>
+      <c r="AH8" s="83"/>
+      <c r="AL8" s="80"/>
+      <c r="AM8" s="81"/>
+      <c r="AN8" s="81"/>
+      <c r="AO8" s="81"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="68" t="s">
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="68" t="s">
+      <c r="F9" s="70"/>
+      <c r="G9" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68" t="s">
+      <c r="H9" s="70"/>
+      <c r="I9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="67"/>
-      <c r="K9" s="68" t="s">
+      <c r="J9" s="70"/>
+      <c r="K9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="67"/>
-      <c r="M9" s="68" t="s">
+      <c r="L9" s="70"/>
+      <c r="M9" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="67"/>
-      <c r="O9" s="75" t="s">
+      <c r="N9" s="70"/>
+      <c r="O9" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="75" t="s">
+      <c r="P9" s="70"/>
+      <c r="Q9" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="67"/>
-      <c r="S9" s="75" t="s">
+      <c r="R9" s="70"/>
+      <c r="S9" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="67"/>
-      <c r="U9" s="75" t="s">
+      <c r="T9" s="70"/>
+      <c r="U9" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="67"/>
-      <c r="W9" s="75" t="s">
+      <c r="V9" s="70"/>
+      <c r="W9" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="67"/>
-      <c r="Y9" s="68" t="s">
+      <c r="X9" s="70"/>
+      <c r="Y9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="67"/>
-      <c r="AA9" s="68" t="s">
+      <c r="Z9" s="70"/>
+      <c r="AA9" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="66" t="s">
+      <c r="AB9" s="70"/>
+      <c r="AC9" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="67"/>
-      <c r="AE9" s="66" t="s">
+      <c r="AD9" s="70"/>
+      <c r="AE9" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="67"/>
-      <c r="AG9" s="66" t="s">
+      <c r="AF9" s="70"/>
+      <c r="AG9" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="67"/>
+      <c r="AH9" s="70"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="68" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="68" t="s">
+      <c r="F10" s="70"/>
+      <c r="G10" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68" t="s">
+      <c r="H10" s="70"/>
+      <c r="I10" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="67"/>
-      <c r="K10" s="68" t="s">
+      <c r="J10" s="70"/>
+      <c r="K10" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="67"/>
-      <c r="M10" s="68" t="s">
+      <c r="L10" s="70"/>
+      <c r="M10" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="67"/>
-      <c r="O10" s="75" t="s">
+      <c r="N10" s="70"/>
+      <c r="O10" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="75" t="s">
+      <c r="P10" s="70"/>
+      <c r="Q10" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="67"/>
-      <c r="S10" s="75" t="s">
+      <c r="R10" s="70"/>
+      <c r="S10" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="67"/>
-      <c r="U10" s="75" t="s">
+      <c r="T10" s="70"/>
+      <c r="U10" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="67"/>
-      <c r="W10" s="75" t="s">
+      <c r="V10" s="70"/>
+      <c r="W10" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="67"/>
-      <c r="Y10" s="68" t="s">
+      <c r="X10" s="70"/>
+      <c r="Y10" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="68" t="s">
+      <c r="Z10" s="70"/>
+      <c r="AA10" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="68" t="s">
+      <c r="AB10" s="70"/>
+      <c r="AC10" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="68" t="s">
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="67"/>
-      <c r="AG10" s="68" t="s">
+      <c r="AF10" s="70"/>
+      <c r="AG10" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="67"/>
+      <c r="AH10" s="70"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1622,11 +1622,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="85" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="65">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1662,9 +1662,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1698,11 +1698,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="85" t="s">
+      <c r="B14" s="68"/>
+      <c r="C14" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="86">
+      <c r="D14" s="65">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1738,9 +1738,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1774,11 +1774,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="85" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="86">
+      <c r="D16" s="65">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1814,9 +1814,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1850,11 +1850,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="85" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="86">
+      <c r="D18" s="65">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1890,9 +1890,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1926,11 +1926,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="85" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="86">
+      <c r="D20" s="65">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1966,9 +1966,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2002,11 +2002,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="85" t="s">
+      <c r="B22" s="62"/>
+      <c r="C22" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="86">
+      <c r="D22" s="65">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2042,9 +2042,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2125,11 +2125,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="85" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="86">
+      <c r="D25" s="65">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2165,9 +2165,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2201,11 +2201,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="85" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="86">
+      <c r="D27" s="65">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2241,9 +2241,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2252,7 +2252,7 @@
       <c r="J28" s="37"/>
       <c r="K28" s="37"/>
       <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
+      <c r="M28" s="59"/>
       <c r="N28" s="37"/>
       <c r="O28" s="38"/>
       <c r="P28" s="38"/>
@@ -2277,11 +2277,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="85" t="s">
+      <c r="B29" s="62"/>
+      <c r="C29" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="86">
+      <c r="D29" s="65">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2317,9 +2317,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2353,11 +2353,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="85" t="s">
+      <c r="B31" s="62"/>
+      <c r="C31" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="86">
+      <c r="D31" s="65">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2393,9 +2393,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2429,11 +2429,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="85" t="s">
+      <c r="B33" s="62"/>
+      <c r="C33" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="86">
+      <c r="D33" s="65">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2468,9 +2468,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2504,11 +2504,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="85" t="s">
+      <c r="B35" s="62"/>
+      <c r="C35" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="86">
+      <c r="D35" s="65">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2543,9 +2543,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="84"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2579,11 +2579,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="85" t="s">
+      <c r="B37" s="62"/>
+      <c r="C37" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="86">
+      <c r="D37" s="65">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2618,9 +2618,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
-      <c r="D38" s="84"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2629,7 +2629,7 @@
       <c r="J38" s="37"/>
       <c r="K38" s="37"/>
       <c r="L38" s="37"/>
-      <c r="M38" s="37"/>
+      <c r="M38" s="59"/>
       <c r="N38" s="37"/>
       <c r="O38" s="42"/>
       <c r="P38" s="42"/>
@@ -2654,11 +2654,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="85" t="s">
+      <c r="B39" s="62"/>
+      <c r="C39" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="86">
+      <c r="D39" s="65">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2693,9 +2693,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="84"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2729,11 +2729,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="83"/>
-      <c r="C41" s="85" t="s">
+      <c r="B41" s="62"/>
+      <c r="C41" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="86">
+      <c r="D41" s="65">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2769,9 +2769,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2852,11 +2852,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="83"/>
-      <c r="C44" s="85" t="s">
+      <c r="B44" s="62"/>
+      <c r="C44" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="86">
+      <c r="D44" s="65">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2892,9 +2892,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2928,11 +2928,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="83"/>
-      <c r="C46" s="85" t="s">
+      <c r="B46" s="62"/>
+      <c r="C46" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="86">
+      <c r="D46" s="65">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2968,17 +2968,17 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="84"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
       <c r="H47" s="59"/>
       <c r="I47" s="59"/>
       <c r="J47" s="59"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="39"/>
+      <c r="K47" s="59"/>
+      <c r="L47" s="59"/>
       <c r="M47" s="39"/>
       <c r="N47" s="39"/>
       <c r="O47" s="38"/>
@@ -3004,11 +3004,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="83"/>
-      <c r="C48" s="85" t="s">
+      <c r="B48" s="62"/>
+      <c r="C48" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="86">
+      <c r="D48" s="65">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3044,18 +3044,18 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="84"/>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
       <c r="H49" s="59"/>
       <c r="I49" s="59"/>
       <c r="J49" s="59"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="37"/>
+      <c r="K49" s="59"/>
+      <c r="L49" s="59"/>
+      <c r="M49" s="59"/>
       <c r="N49" s="37"/>
       <c r="O49" s="43"/>
       <c r="P49" s="43"/>
@@ -3086,16 +3086,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="88"/>
-      <c r="F50" s="79"/>
-      <c r="G50" s="88"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="88"/>
-      <c r="J50" s="79"/>
-      <c r="K50" s="88"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="88"/>
-      <c r="N50" s="79"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="66"/>
+      <c r="L50" s="67"/>
+      <c r="M50" s="66"/>
+      <c r="N50" s="67"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3106,10 +3106,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="88"/>
-      <c r="Z50" s="79"/>
-      <c r="AA50" s="88"/>
-      <c r="AB50" s="79"/>
+      <c r="Y50" s="66"/>
+      <c r="Z50" s="67"/>
+      <c r="AA50" s="66"/>
+      <c r="AB50" s="67"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3183,43 +3183,52 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="Y8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
@@ -3244,52 +3253,43 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="Y8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modification du pdf pour ajouter les heures totales
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -778,6 +778,55 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -788,60 +837,11 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,8 +1135,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1184,17 +1184,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1258,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="72"/>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="73" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="72"/>
@@ -1279,7 +1279,7 @@
       <c r="R4" s="72"/>
       <c r="S4" s="72"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="88" t="s">
+      <c r="U4" s="74" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="72"/>
@@ -1295,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="72"/>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="76" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="72"/>
@@ -1316,7 +1316,7 @@
       <c r="R5" s="72"/>
       <c r="S5" s="72"/>
       <c r="T5" s="72"/>
-      <c r="U5" s="74">
+      <c r="U5" s="77">
         <v>44319</v>
       </c>
       <c r="V5" s="72"/>
@@ -1388,187 +1388,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="76" t="s">
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="77"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="77"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="82" t="s">
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="81"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="83"/>
-      <c r="AA8" s="83"/>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83"/>
-      <c r="AE8" s="83"/>
-      <c r="AF8" s="83"/>
-      <c r="AG8" s="83"/>
-      <c r="AH8" s="83"/>
-      <c r="AL8" s="80"/>
-      <c r="AM8" s="81"/>
-      <c r="AN8" s="81"/>
-      <c r="AO8" s="81"/>
+      <c r="Z8" s="65"/>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="65"/>
+      <c r="AE8" s="65"/>
+      <c r="AF8" s="65"/>
+      <c r="AG8" s="65"/>
+      <c r="AH8" s="65"/>
+      <c r="AL8" s="62"/>
+      <c r="AM8" s="63"/>
+      <c r="AN8" s="63"/>
+      <c r="AO8" s="63"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="69" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="69" t="s">
+      <c r="F9" s="67"/>
+      <c r="G9" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="70"/>
-      <c r="I9" s="69" t="s">
+      <c r="H9" s="67"/>
+      <c r="I9" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="70"/>
-      <c r="K9" s="69" t="s">
+      <c r="J9" s="67"/>
+      <c r="K9" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="70"/>
-      <c r="M9" s="69" t="s">
+      <c r="L9" s="67"/>
+      <c r="M9" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="70"/>
-      <c r="O9" s="79" t="s">
+      <c r="N9" s="67"/>
+      <c r="O9" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="79" t="s">
+      <c r="P9" s="67"/>
+      <c r="Q9" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="70"/>
-      <c r="S9" s="79" t="s">
+      <c r="R9" s="67"/>
+      <c r="S9" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="70"/>
-      <c r="U9" s="79" t="s">
+      <c r="T9" s="67"/>
+      <c r="U9" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="70"/>
-      <c r="W9" s="79" t="s">
+      <c r="V9" s="67"/>
+      <c r="W9" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="69" t="s">
+      <c r="X9" s="67"/>
+      <c r="Y9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="69" t="s">
+      <c r="Z9" s="67"/>
+      <c r="AA9" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="70"/>
-      <c r="AC9" s="84" t="s">
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="70"/>
-      <c r="AE9" s="84" t="s">
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="70"/>
-      <c r="AG9" s="84" t="s">
+      <c r="AF9" s="67"/>
+      <c r="AG9" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="70"/>
+      <c r="AH9" s="67"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="69" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="70"/>
-      <c r="G10" s="69" t="s">
+      <c r="F10" s="67"/>
+      <c r="G10" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="70"/>
-      <c r="I10" s="69" t="s">
+      <c r="H10" s="67"/>
+      <c r="I10" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="70"/>
-      <c r="K10" s="69" t="s">
+      <c r="J10" s="67"/>
+      <c r="K10" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="70"/>
-      <c r="M10" s="69" t="s">
+      <c r="L10" s="67"/>
+      <c r="M10" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="70"/>
-      <c r="O10" s="79" t="s">
+      <c r="N10" s="67"/>
+      <c r="O10" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="79" t="s">
+      <c r="P10" s="67"/>
+      <c r="Q10" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="70"/>
-      <c r="S10" s="79" t="s">
+      <c r="R10" s="67"/>
+      <c r="S10" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="70"/>
-      <c r="U10" s="79" t="s">
+      <c r="T10" s="67"/>
+      <c r="U10" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="70"/>
-      <c r="W10" s="79" t="s">
+      <c r="V10" s="67"/>
+      <c r="W10" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="70"/>
-      <c r="Y10" s="69" t="s">
+      <c r="X10" s="67"/>
+      <c r="Y10" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="69" t="s">
+      <c r="Z10" s="67"/>
+      <c r="AA10" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="70"/>
-      <c r="AC10" s="69" t="s">
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="70"/>
-      <c r="AE10" s="69" t="s">
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="70"/>
-      <c r="AG10" s="69" t="s">
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="70"/>
+      <c r="AH10" s="67"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1622,11 +1622,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="64" t="s">
+      <c r="B12" s="83"/>
+      <c r="C12" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="86">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1662,9 +1662,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1698,11 +1698,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="64" t="s">
+      <c r="B14" s="87"/>
+      <c r="C14" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="86">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1738,9 +1738,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1774,11 +1774,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="83"/>
+      <c r="C16" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="86">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1814,9 +1814,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1850,11 +1850,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="64" t="s">
+      <c r="B18" s="83"/>
+      <c r="C18" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="86">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1890,9 +1890,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1926,11 +1926,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="83"/>
+      <c r="C20" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="86">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1966,9 +1966,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2002,11 +2002,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="83"/>
+      <c r="C22" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="86">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2042,9 +2042,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2125,11 +2125,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="64" t="s">
+      <c r="B25" s="83"/>
+      <c r="C25" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="86">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2165,9 +2165,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2201,11 +2201,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="83"/>
+      <c r="C27" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="86">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2241,9 +2241,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2277,11 +2277,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="64" t="s">
+      <c r="B29" s="83"/>
+      <c r="C29" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="86">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2317,9 +2317,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2353,11 +2353,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="64" t="s">
+      <c r="B31" s="83"/>
+      <c r="C31" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="86">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2393,9 +2393,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2429,11 +2429,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="64" t="s">
+      <c r="B33" s="83"/>
+      <c r="C33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="86">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2468,9 +2468,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2504,11 +2504,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="64" t="s">
+      <c r="B35" s="83"/>
+      <c r="C35" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="86">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2543,9 +2543,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2579,11 +2579,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="64" t="s">
+      <c r="B37" s="83"/>
+      <c r="C37" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="86">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2618,9 +2618,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="84"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2654,11 +2654,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="64" t="s">
+      <c r="B39" s="83"/>
+      <c r="C39" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="86">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2693,9 +2693,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2729,11 +2729,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="64" t="s">
+      <c r="B41" s="83"/>
+      <c r="C41" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="86">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2769,9 +2769,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2852,11 +2852,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="64" t="s">
+      <c r="B44" s="83"/>
+      <c r="C44" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="86">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2892,9 +2892,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2928,11 +2928,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="64" t="s">
+      <c r="B46" s="83"/>
+      <c r="C46" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="86">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2968,9 +2968,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -2979,7 +2979,7 @@
       <c r="J47" s="59"/>
       <c r="K47" s="59"/>
       <c r="L47" s="59"/>
-      <c r="M47" s="39"/>
+      <c r="M47" s="59"/>
       <c r="N47" s="39"/>
       <c r="O47" s="38"/>
       <c r="P47" s="38"/>
@@ -3004,11 +3004,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="64" t="s">
+      <c r="B48" s="83"/>
+      <c r="C48" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="65">
+      <c r="D48" s="86">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3044,9 +3044,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3086,16 +3086,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="66"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="67"/>
-      <c r="K50" s="66"/>
-      <c r="L50" s="67"/>
-      <c r="M50" s="66"/>
-      <c r="N50" s="67"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="88"/>
+      <c r="J50" s="79"/>
+      <c r="K50" s="88"/>
+      <c r="L50" s="79"/>
+      <c r="M50" s="88"/>
+      <c r="N50" s="79"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3106,10 +3106,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="66"/>
-      <c r="Z50" s="67"/>
-      <c r="AA50" s="66"/>
-      <c r="AB50" s="67"/>
+      <c r="Y50" s="88"/>
+      <c r="Z50" s="79"/>
+      <c r="AA50" s="88"/>
+      <c r="AB50" s="79"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3183,6 +3183,89 @@
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="AL8:AO8"/>
     <mergeCell ref="Y8:AH8"/>
     <mergeCell ref="AC9:AD9"/>
@@ -3207,89 +3290,6 @@
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout de boutons pour télécharger les données
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -390,7 +390,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,6 +473,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2F4152"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2F4152"/>
+        <bgColor rgb="FFDDEBF7"/>
       </patternFill>
     </fill>
   </fills>
@@ -603,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -778,55 +784,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -837,10 +794,65 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1135,8 +1147,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AB33" sqref="AB33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1184,17 +1196,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1258,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="72"/>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="87" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="72"/>
@@ -1279,7 +1291,7 @@
       <c r="R4" s="72"/>
       <c r="S4" s="72"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="88" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="72"/>
@@ -1295,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="72"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="73" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="72"/>
@@ -1316,7 +1328,7 @@
       <c r="R5" s="72"/>
       <c r="S5" s="72"/>
       <c r="T5" s="72"/>
-      <c r="U5" s="77">
+      <c r="U5" s="74">
         <v>44319</v>
       </c>
       <c r="V5" s="72"/>
@@ -1388,187 +1400,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="80" t="s">
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="81"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="81"/>
-      <c r="V8" s="81"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="82"/>
-      <c r="Y8" s="64" t="s">
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="77"/>
+      <c r="T8" s="77"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="78"/>
+      <c r="Y8" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="65"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="65"/>
-      <c r="AD8" s="65"/>
-      <c r="AE8" s="65"/>
-      <c r="AF8" s="65"/>
-      <c r="AG8" s="65"/>
-      <c r="AH8" s="65"/>
-      <c r="AL8" s="62"/>
-      <c r="AM8" s="63"/>
-      <c r="AN8" s="63"/>
-      <c r="AO8" s="63"/>
+      <c r="Z8" s="83"/>
+      <c r="AA8" s="83"/>
+      <c r="AB8" s="83"/>
+      <c r="AC8" s="83"/>
+      <c r="AD8" s="83"/>
+      <c r="AE8" s="83"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="83"/>
+      <c r="AH8" s="83"/>
+      <c r="AL8" s="80"/>
+      <c r="AM8" s="81"/>
+      <c r="AN8" s="81"/>
+      <c r="AO8" s="81"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="68" t="s">
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="68" t="s">
+      <c r="F9" s="70"/>
+      <c r="G9" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68" t="s">
+      <c r="H9" s="70"/>
+      <c r="I9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="67"/>
-      <c r="K9" s="68" t="s">
+      <c r="J9" s="70"/>
+      <c r="K9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="67"/>
-      <c r="M9" s="68" t="s">
+      <c r="L9" s="70"/>
+      <c r="M9" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="67"/>
-      <c r="O9" s="75" t="s">
+      <c r="N9" s="70"/>
+      <c r="O9" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="75" t="s">
+      <c r="P9" s="70"/>
+      <c r="Q9" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="67"/>
-      <c r="S9" s="75" t="s">
+      <c r="R9" s="70"/>
+      <c r="S9" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="67"/>
-      <c r="U9" s="75" t="s">
+      <c r="T9" s="70"/>
+      <c r="U9" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="67"/>
-      <c r="W9" s="75" t="s">
+      <c r="V9" s="70"/>
+      <c r="W9" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="67"/>
-      <c r="Y9" s="68" t="s">
+      <c r="X9" s="70"/>
+      <c r="Y9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="67"/>
-      <c r="AA9" s="68" t="s">
+      <c r="Z9" s="70"/>
+      <c r="AA9" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="66" t="s">
+      <c r="AB9" s="70"/>
+      <c r="AC9" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="67"/>
-      <c r="AE9" s="66" t="s">
+      <c r="AD9" s="70"/>
+      <c r="AE9" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="67"/>
-      <c r="AG9" s="66" t="s">
+      <c r="AF9" s="70"/>
+      <c r="AG9" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="67"/>
+      <c r="AH9" s="70"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="68" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="68" t="s">
+      <c r="F10" s="70"/>
+      <c r="G10" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68" t="s">
+      <c r="H10" s="70"/>
+      <c r="I10" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="67"/>
-      <c r="K10" s="68" t="s">
+      <c r="J10" s="70"/>
+      <c r="K10" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="67"/>
-      <c r="M10" s="68" t="s">
+      <c r="L10" s="70"/>
+      <c r="M10" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="67"/>
-      <c r="O10" s="75" t="s">
+      <c r="N10" s="70"/>
+      <c r="O10" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="75" t="s">
+      <c r="P10" s="70"/>
+      <c r="Q10" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="67"/>
-      <c r="S10" s="75" t="s">
+      <c r="R10" s="70"/>
+      <c r="S10" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="67"/>
-      <c r="U10" s="75" t="s">
+      <c r="T10" s="70"/>
+      <c r="U10" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="67"/>
-      <c r="W10" s="75" t="s">
+      <c r="V10" s="70"/>
+      <c r="W10" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="67"/>
-      <c r="Y10" s="68" t="s">
+      <c r="X10" s="70"/>
+      <c r="Y10" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="68" t="s">
+      <c r="Z10" s="70"/>
+      <c r="AA10" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="68" t="s">
+      <c r="AB10" s="70"/>
+      <c r="AC10" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="68" t="s">
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="67"/>
-      <c r="AG10" s="68" t="s">
+      <c r="AF10" s="70"/>
+      <c r="AG10" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="67"/>
+      <c r="AH10" s="70"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1622,11 +1634,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="85" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="65">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1662,9 +1674,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1698,11 +1710,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="85" t="s">
+      <c r="B14" s="68"/>
+      <c r="C14" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="86">
+      <c r="D14" s="65">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1738,9 +1750,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1774,11 +1786,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="85" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="86">
+      <c r="D16" s="65">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1814,9 +1826,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1850,11 +1862,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="85" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="86">
+      <c r="D18" s="65">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1890,9 +1902,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1926,11 +1938,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="85" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="86">
+      <c r="D20" s="65">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1966,9 +1978,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2002,11 +2014,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="85" t="s">
+      <c r="B22" s="62"/>
+      <c r="C22" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="86">
+      <c r="D22" s="65">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2042,9 +2054,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2125,11 +2137,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="85" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="86">
+      <c r="D25" s="65">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2165,9 +2177,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2201,11 +2213,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="85" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="86">
+      <c r="D27" s="65">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2241,9 +2253,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2277,11 +2289,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="85" t="s">
+      <c r="B29" s="62"/>
+      <c r="C29" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="86">
+      <c r="D29" s="65">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2317,9 +2329,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2353,11 +2365,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="85" t="s">
+      <c r="B31" s="62"/>
+      <c r="C31" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="86">
+      <c r="D31" s="65">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2393,9 +2405,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2429,11 +2441,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="85" t="s">
+      <c r="B33" s="62"/>
+      <c r="C33" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="86">
+      <c r="D33" s="65">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2468,9 +2480,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2504,11 +2516,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="85" t="s">
+      <c r="B35" s="62"/>
+      <c r="C35" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="86">
+      <c r="D35" s="65">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2543,9 +2555,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="84"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2579,11 +2591,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="85" t="s">
+      <c r="B37" s="62"/>
+      <c r="C37" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="86">
+      <c r="D37" s="65">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2618,9 +2630,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
-      <c r="D38" s="84"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2631,7 +2643,7 @@
       <c r="L38" s="37"/>
       <c r="M38" s="59"/>
       <c r="N38" s="37"/>
-      <c r="O38" s="42"/>
+      <c r="O38" s="89"/>
       <c r="P38" s="42"/>
       <c r="Q38" s="42"/>
       <c r="R38" s="43"/>
@@ -2654,11 +2666,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="85" t="s">
+      <c r="B39" s="62"/>
+      <c r="C39" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="86">
+      <c r="D39" s="65">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2693,9 +2705,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="84"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2729,11 +2741,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="83"/>
-      <c r="C41" s="85" t="s">
+      <c r="B41" s="62"/>
+      <c r="C41" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="86">
+      <c r="D41" s="65">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2769,9 +2781,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2852,11 +2864,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="83"/>
-      <c r="C44" s="85" t="s">
+      <c r="B44" s="62"/>
+      <c r="C44" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="86">
+      <c r="D44" s="65">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2892,9 +2904,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2928,11 +2940,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="83"/>
-      <c r="C46" s="85" t="s">
+      <c r="B46" s="62"/>
+      <c r="C46" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="86">
+      <c r="D46" s="65">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2968,9 +2980,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="84"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -2981,7 +2993,7 @@
       <c r="L47" s="59"/>
       <c r="M47" s="59"/>
       <c r="N47" s="39"/>
-      <c r="O47" s="38"/>
+      <c r="O47" s="89"/>
       <c r="P47" s="38"/>
       <c r="Q47" s="43"/>
       <c r="R47" s="38"/>
@@ -3004,11 +3016,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="83"/>
-      <c r="C48" s="85" t="s">
+      <c r="B48" s="62"/>
+      <c r="C48" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="86">
+      <c r="D48" s="65">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3044,9 +3056,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="84"/>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3057,7 +3069,7 @@
       <c r="L49" s="59"/>
       <c r="M49" s="59"/>
       <c r="N49" s="37"/>
-      <c r="O49" s="43"/>
+      <c r="O49" s="90"/>
       <c r="P49" s="43"/>
       <c r="Q49" s="43"/>
       <c r="R49" s="43"/>
@@ -3086,16 +3098,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="88"/>
-      <c r="F50" s="79"/>
-      <c r="G50" s="88"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="88"/>
-      <c r="J50" s="79"/>
-      <c r="K50" s="88"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="88"/>
-      <c r="N50" s="79"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="66"/>
+      <c r="L50" s="67"/>
+      <c r="M50" s="66"/>
+      <c r="N50" s="67"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3106,10 +3118,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="88"/>
-      <c r="Z50" s="79"/>
-      <c r="AA50" s="88"/>
-      <c r="AB50" s="79"/>
+      <c r="Y50" s="66"/>
+      <c r="Z50" s="67"/>
+      <c r="AA50" s="66"/>
+      <c r="AB50" s="67"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3183,43 +3195,52 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="Y8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
@@ -3244,52 +3265,43 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="Y8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
doc + typo dans la doc
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -784,6 +784,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -794,65 +849,10 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1147,8 +1147,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AB33" sqref="AB33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1196,17 +1196,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1266,77 +1266,77 @@
     </row>
     <row r="4" spans="1:41" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="87" t="s">
+      <c r="C4" s="74"/>
+      <c r="D4" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="15"/>
-      <c r="L4" s="71" t="s">
+      <c r="L4" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="72"/>
-      <c r="U4" s="88" t="s">
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="V4" s="72"/>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
     </row>
     <row r="5" spans="1:41" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73" t="s">
+      <c r="C5" s="74"/>
+      <c r="D5" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="15"/>
-      <c r="L5" s="71" t="s">
+      <c r="L5" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="74">
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="79">
         <v>44319</v>
       </c>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="72"/>
-      <c r="Y5" s="72"/>
-      <c r="Z5" s="72"/>
-      <c r="AA5" s="72"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
     </row>
     <row r="6" spans="1:41" ht="21" customHeight="1">
       <c r="A6" s="17"/>
@@ -1400,187 +1400,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="76" t="s">
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="84"/>
+      <c r="O8" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="77"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="77"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="82" t="s">
+      <c r="P8" s="83"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="83"/>
+      <c r="S8" s="83"/>
+      <c r="T8" s="83"/>
+      <c r="U8" s="83"/>
+      <c r="V8" s="83"/>
+      <c r="W8" s="83"/>
+      <c r="X8" s="84"/>
+      <c r="Y8" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="83"/>
-      <c r="AA8" s="83"/>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83"/>
-      <c r="AE8" s="83"/>
-      <c r="AF8" s="83"/>
-      <c r="AG8" s="83"/>
-      <c r="AH8" s="83"/>
-      <c r="AL8" s="80"/>
-      <c r="AM8" s="81"/>
-      <c r="AN8" s="81"/>
-      <c r="AO8" s="81"/>
+      <c r="Z8" s="67"/>
+      <c r="AA8" s="67"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
+      <c r="AE8" s="67"/>
+      <c r="AF8" s="67"/>
+      <c r="AG8" s="67"/>
+      <c r="AH8" s="67"/>
+      <c r="AL8" s="64"/>
+      <c r="AM8" s="65"/>
+      <c r="AN8" s="65"/>
+      <c r="AO8" s="65"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="69" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="69" t="s">
+      <c r="F9" s="69"/>
+      <c r="G9" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="70"/>
-      <c r="I9" s="69" t="s">
+      <c r="H9" s="69"/>
+      <c r="I9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="70"/>
-      <c r="K9" s="69" t="s">
+      <c r="J9" s="69"/>
+      <c r="K9" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="70"/>
-      <c r="M9" s="69" t="s">
+      <c r="L9" s="69"/>
+      <c r="M9" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="70"/>
-      <c r="O9" s="79" t="s">
+      <c r="N9" s="69"/>
+      <c r="O9" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="79" t="s">
+      <c r="P9" s="69"/>
+      <c r="Q9" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="70"/>
-      <c r="S9" s="79" t="s">
+      <c r="R9" s="69"/>
+      <c r="S9" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="70"/>
-      <c r="U9" s="79" t="s">
+      <c r="T9" s="69"/>
+      <c r="U9" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="70"/>
-      <c r="W9" s="79" t="s">
+      <c r="V9" s="69"/>
+      <c r="W9" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="69" t="s">
+      <c r="X9" s="69"/>
+      <c r="Y9" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="69" t="s">
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="70"/>
-      <c r="AC9" s="84" t="s">
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="70"/>
-      <c r="AE9" s="84" t="s">
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="70"/>
-      <c r="AG9" s="84" t="s">
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="70"/>
+      <c r="AH9" s="69"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="69" t="s">
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="70"/>
-      <c r="G10" s="69" t="s">
+      <c r="F10" s="69"/>
+      <c r="G10" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="70"/>
-      <c r="I10" s="69" t="s">
+      <c r="H10" s="69"/>
+      <c r="I10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="70"/>
-      <c r="K10" s="69" t="s">
+      <c r="J10" s="69"/>
+      <c r="K10" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="70"/>
-      <c r="M10" s="69" t="s">
+      <c r="L10" s="69"/>
+      <c r="M10" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="70"/>
-      <c r="O10" s="79" t="s">
+      <c r="N10" s="69"/>
+      <c r="O10" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="79" t="s">
+      <c r="P10" s="69"/>
+      <c r="Q10" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="70"/>
-      <c r="S10" s="79" t="s">
+      <c r="R10" s="69"/>
+      <c r="S10" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="70"/>
-      <c r="U10" s="79" t="s">
+      <c r="T10" s="69"/>
+      <c r="U10" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="70"/>
-      <c r="W10" s="79" t="s">
+      <c r="V10" s="69"/>
+      <c r="W10" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="70"/>
-      <c r="Y10" s="69" t="s">
+      <c r="X10" s="69"/>
+      <c r="Y10" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="69" t="s">
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="70"/>
-      <c r="AC10" s="69" t="s">
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="70"/>
-      <c r="AE10" s="69" t="s">
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="70"/>
-      <c r="AG10" s="69" t="s">
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="70"/>
+      <c r="AH10" s="69"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1634,11 +1634,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="64" t="s">
+      <c r="B12" s="85"/>
+      <c r="C12" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="88">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1674,9 +1674,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1710,11 +1710,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="64" t="s">
+      <c r="B14" s="89"/>
+      <c r="C14" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="88">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1750,9 +1750,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1786,11 +1786,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="85"/>
+      <c r="C16" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="88">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1826,9 +1826,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1862,11 +1862,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="64" t="s">
+      <c r="B18" s="85"/>
+      <c r="C18" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="88">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1902,9 +1902,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1938,11 +1938,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="85"/>
+      <c r="C20" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="88">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1978,9 +1978,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2014,11 +2014,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="85"/>
+      <c r="C22" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="88">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2054,9 +2054,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2137,11 +2137,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="64" t="s">
+      <c r="B25" s="85"/>
+      <c r="C25" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="88">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2177,9 +2177,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2213,11 +2213,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="85"/>
+      <c r="C27" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="88">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2253,9 +2253,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2289,11 +2289,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="64" t="s">
+      <c r="B29" s="85"/>
+      <c r="C29" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="88">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2329,9 +2329,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="86"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2365,11 +2365,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="64" t="s">
+      <c r="B31" s="85"/>
+      <c r="C31" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="88">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2405,9 +2405,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2441,11 +2441,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="64" t="s">
+      <c r="B33" s="85"/>
+      <c r="C33" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="88">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2480,9 +2480,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2516,11 +2516,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="64" t="s">
+      <c r="B35" s="85"/>
+      <c r="C35" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="88">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2555,9 +2555,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
+      <c r="B36" s="86"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2591,11 +2591,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="64" t="s">
+      <c r="B37" s="85"/>
+      <c r="C37" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="88">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2630,9 +2630,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2643,7 +2643,7 @@
       <c r="L38" s="37"/>
       <c r="M38" s="59"/>
       <c r="N38" s="37"/>
-      <c r="O38" s="89"/>
+      <c r="O38" s="62"/>
       <c r="P38" s="42"/>
       <c r="Q38" s="42"/>
       <c r="R38" s="43"/>
@@ -2666,11 +2666,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="64" t="s">
+      <c r="B39" s="85"/>
+      <c r="C39" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="88">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2705,9 +2705,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2719,7 +2719,7 @@
       <c r="M40" s="55"/>
       <c r="N40" s="55"/>
       <c r="O40" s="42"/>
-      <c r="P40" s="42"/>
+      <c r="P40" s="62"/>
       <c r="Q40" s="43"/>
       <c r="R40" s="42"/>
       <c r="S40" s="42"/>
@@ -2741,11 +2741,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="64" t="s">
+      <c r="B41" s="85"/>
+      <c r="C41" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="65">
+      <c r="D41" s="88">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2781,9 +2781,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2864,11 +2864,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="64" t="s">
+      <c r="B44" s="85"/>
+      <c r="C44" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="88">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2904,9 +2904,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2940,11 +2940,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="64" t="s">
+      <c r="B46" s="85"/>
+      <c r="C46" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="88">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2980,9 +2980,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -2993,8 +2993,8 @@
       <c r="L47" s="59"/>
       <c r="M47" s="59"/>
       <c r="N47" s="39"/>
-      <c r="O47" s="89"/>
-      <c r="P47" s="38"/>
+      <c r="O47" s="62"/>
+      <c r="P47" s="62"/>
       <c r="Q47" s="43"/>
       <c r="R47" s="38"/>
       <c r="S47" s="38"/>
@@ -3016,11 +3016,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="64" t="s">
+      <c r="B48" s="85"/>
+      <c r="C48" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="65">
+      <c r="D48" s="88">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3056,9 +3056,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="86"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3069,8 +3069,8 @@
       <c r="L49" s="59"/>
       <c r="M49" s="59"/>
       <c r="N49" s="37"/>
-      <c r="O49" s="90"/>
-      <c r="P49" s="43"/>
+      <c r="O49" s="63"/>
+      <c r="P49" s="63"/>
       <c r="Q49" s="43"/>
       <c r="R49" s="43"/>
       <c r="S49" s="43"/>
@@ -3098,16 +3098,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="66"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="67"/>
-      <c r="K50" s="66"/>
-      <c r="L50" s="67"/>
-      <c r="M50" s="66"/>
-      <c r="N50" s="67"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="81"/>
+      <c r="I50" s="90"/>
+      <c r="J50" s="81"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="81"/>
+      <c r="M50" s="90"/>
+      <c r="N50" s="81"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3118,10 +3118,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="66"/>
-      <c r="Z50" s="67"/>
-      <c r="AA50" s="66"/>
-      <c r="AB50" s="67"/>
+      <c r="Y50" s="90"/>
+      <c r="Z50" s="81"/>
+      <c r="AA50" s="90"/>
+      <c r="AB50" s="81"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3195,6 +3195,89 @@
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="AL8:AO8"/>
     <mergeCell ref="Y8:AH8"/>
     <mergeCell ref="AC9:AD9"/>
@@ -3219,89 +3302,6 @@
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modification de vol fonctionnel
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -790,55 +790,6 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -849,11 +800,60 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,8 +1147,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1196,17 +1196,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="74"/>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="89" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74"/>
@@ -1291,7 +1291,7 @@
       <c r="R4" s="74"/>
       <c r="S4" s="74"/>
       <c r="T4" s="74"/>
-      <c r="U4" s="76" t="s">
+      <c r="U4" s="90" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="74"/>
@@ -1307,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="74"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="75" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="74"/>
@@ -1328,7 +1328,7 @@
       <c r="R5" s="74"/>
       <c r="S5" s="74"/>
       <c r="T5" s="74"/>
-      <c r="U5" s="79">
+      <c r="U5" s="76">
         <v>44319</v>
       </c>
       <c r="V5" s="74"/>
@@ -1400,187 +1400,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="82" t="s">
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="84"/>
-      <c r="Y8" s="66" t="s">
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="79"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="79"/>
+      <c r="X8" s="80"/>
+      <c r="Y8" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="67"/>
-      <c r="AA8" s="67"/>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="67"/>
-      <c r="AG8" s="67"/>
-      <c r="AH8" s="67"/>
-      <c r="AL8" s="64"/>
-      <c r="AM8" s="65"/>
-      <c r="AN8" s="65"/>
-      <c r="AO8" s="65"/>
+      <c r="Z8" s="85"/>
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="85"/>
+      <c r="AC8" s="85"/>
+      <c r="AD8" s="85"/>
+      <c r="AE8" s="85"/>
+      <c r="AF8" s="85"/>
+      <c r="AG8" s="85"/>
+      <c r="AH8" s="85"/>
+      <c r="AL8" s="82"/>
+      <c r="AM8" s="83"/>
+      <c r="AN8" s="83"/>
+      <c r="AO8" s="83"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="70" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70" t="s">
+      <c r="F9" s="72"/>
+      <c r="G9" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70" t="s">
+      <c r="H9" s="72"/>
+      <c r="I9" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="70" t="s">
+      <c r="J9" s="72"/>
+      <c r="K9" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="69"/>
-      <c r="M9" s="70" t="s">
+      <c r="L9" s="72"/>
+      <c r="M9" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="69"/>
-      <c r="O9" s="77" t="s">
+      <c r="N9" s="72"/>
+      <c r="O9" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="77" t="s">
+      <c r="P9" s="72"/>
+      <c r="Q9" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="69"/>
-      <c r="S9" s="77" t="s">
+      <c r="R9" s="72"/>
+      <c r="S9" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="69"/>
-      <c r="U9" s="77" t="s">
+      <c r="T9" s="72"/>
+      <c r="U9" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="69"/>
-      <c r="W9" s="77" t="s">
+      <c r="V9" s="72"/>
+      <c r="W9" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="69"/>
-      <c r="Y9" s="70" t="s">
+      <c r="X9" s="72"/>
+      <c r="Y9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="70" t="s">
+      <c r="Z9" s="72"/>
+      <c r="AA9" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="68" t="s">
+      <c r="AB9" s="72"/>
+      <c r="AC9" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="68" t="s">
+      <c r="AD9" s="72"/>
+      <c r="AE9" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="68" t="s">
+      <c r="AF9" s="72"/>
+      <c r="AG9" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="69"/>
+      <c r="AH9" s="72"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="70" t="s">
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="70" t="s">
+      <c r="F10" s="72"/>
+      <c r="G10" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="69"/>
-      <c r="I10" s="70" t="s">
+      <c r="H10" s="72"/>
+      <c r="I10" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70" t="s">
+      <c r="J10" s="72"/>
+      <c r="K10" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="69"/>
-      <c r="M10" s="70" t="s">
+      <c r="L10" s="72"/>
+      <c r="M10" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="69"/>
-      <c r="O10" s="77" t="s">
+      <c r="N10" s="72"/>
+      <c r="O10" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="77" t="s">
+      <c r="P10" s="72"/>
+      <c r="Q10" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="69"/>
-      <c r="S10" s="77" t="s">
+      <c r="R10" s="72"/>
+      <c r="S10" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="69"/>
-      <c r="U10" s="77" t="s">
+      <c r="T10" s="72"/>
+      <c r="U10" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="69"/>
-      <c r="W10" s="77" t="s">
+      <c r="V10" s="72"/>
+      <c r="W10" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="69"/>
-      <c r="Y10" s="70" t="s">
+      <c r="X10" s="72"/>
+      <c r="Y10" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="70" t="s">
+      <c r="Z10" s="72"/>
+      <c r="AA10" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="70" t="s">
+      <c r="AB10" s="72"/>
+      <c r="AC10" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="70" t="s">
+      <c r="AD10" s="72"/>
+      <c r="AE10" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="70" t="s">
+      <c r="AF10" s="72"/>
+      <c r="AG10" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="69"/>
+      <c r="AH10" s="72"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1634,11 +1634,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="87" t="s">
+      <c r="B12" s="64"/>
+      <c r="C12" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="88">
+      <c r="D12" s="67">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1674,9 +1674,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1710,11 +1710,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="87" t="s">
+      <c r="B14" s="70"/>
+      <c r="C14" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="88">
+      <c r="D14" s="67">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1750,9 +1750,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1786,11 +1786,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="87" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="88">
+      <c r="D16" s="67">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1826,9 +1826,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1862,11 +1862,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="87" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="88">
+      <c r="D18" s="67">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1902,9 +1902,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1938,11 +1938,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="87" t="s">
+      <c r="B20" s="64"/>
+      <c r="C20" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="88">
+      <c r="D20" s="67">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1978,9 +1978,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2014,11 +2014,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="87" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="88">
+      <c r="D22" s="67">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2054,9 +2054,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2137,11 +2137,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="87" t="s">
+      <c r="B25" s="64"/>
+      <c r="C25" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="88">
+      <c r="D25" s="67">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2177,9 +2177,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2213,11 +2213,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="87" t="s">
+      <c r="B27" s="64"/>
+      <c r="C27" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="88">
+      <c r="D27" s="67">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2253,9 +2253,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2289,11 +2289,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="87" t="s">
+      <c r="B29" s="64"/>
+      <c r="C29" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="88">
+      <c r="D29" s="67">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2329,9 +2329,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2365,11 +2365,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="87" t="s">
+      <c r="B31" s="64"/>
+      <c r="C31" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="88">
+      <c r="D31" s="67">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2405,9 +2405,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2441,11 +2441,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="87" t="s">
+      <c r="B33" s="64"/>
+      <c r="C33" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="88">
+      <c r="D33" s="67">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2480,9 +2480,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2516,11 +2516,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="87" t="s">
+      <c r="B35" s="64"/>
+      <c r="C35" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="88">
+      <c r="D35" s="67">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2555,9 +2555,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2591,11 +2591,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="87" t="s">
+      <c r="B37" s="64"/>
+      <c r="C37" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="88">
+      <c r="D37" s="67">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2630,9 +2630,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2666,11 +2666,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="87" t="s">
+      <c r="B39" s="64"/>
+      <c r="C39" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="88">
+      <c r="D39" s="67">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2705,9 +2705,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2720,7 +2720,7 @@
       <c r="N40" s="55"/>
       <c r="O40" s="42"/>
       <c r="P40" s="62"/>
-      <c r="Q40" s="43"/>
+      <c r="Q40" s="63"/>
       <c r="R40" s="42"/>
       <c r="S40" s="42"/>
       <c r="T40" s="42"/>
@@ -2741,11 +2741,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="87" t="s">
+      <c r="B41" s="64"/>
+      <c r="C41" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="88">
+      <c r="D41" s="67">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2781,9 +2781,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2864,11 +2864,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="85"/>
-      <c r="C44" s="87" t="s">
+      <c r="B44" s="64"/>
+      <c r="C44" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="88">
+      <c r="D44" s="67">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2904,9 +2904,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="86"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2940,11 +2940,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="85"/>
-      <c r="C46" s="87" t="s">
+      <c r="B46" s="64"/>
+      <c r="C46" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="88">
+      <c r="D46" s="67">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2980,9 +2980,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="86"/>
-      <c r="C47" s="86"/>
-      <c r="D47" s="86"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -2995,7 +2995,7 @@
       <c r="N47" s="39"/>
       <c r="O47" s="62"/>
       <c r="P47" s="62"/>
-      <c r="Q47" s="43"/>
+      <c r="Q47" s="63"/>
       <c r="R47" s="38"/>
       <c r="S47" s="38"/>
       <c r="T47" s="38"/>
@@ -3016,11 +3016,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="85"/>
-      <c r="C48" s="87" t="s">
+      <c r="B48" s="64"/>
+      <c r="C48" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="88">
+      <c r="D48" s="67">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3056,9 +3056,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="86"/>
-      <c r="D49" s="86"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3071,7 +3071,7 @@
       <c r="N49" s="37"/>
       <c r="O49" s="63"/>
       <c r="P49" s="63"/>
-      <c r="Q49" s="43"/>
+      <c r="Q49" s="63"/>
       <c r="R49" s="43"/>
       <c r="S49" s="43"/>
       <c r="T49" s="43"/>
@@ -3098,16 +3098,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="90"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="81"/>
-      <c r="M50" s="90"/>
-      <c r="N50" s="81"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="68"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="68"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="69"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3118,10 +3118,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="90"/>
-      <c r="Z50" s="81"/>
-      <c r="AA50" s="90"/>
-      <c r="AB50" s="81"/>
+      <c r="Y50" s="68"/>
+      <c r="Z50" s="69"/>
+      <c r="AA50" s="68"/>
+      <c r="AB50" s="69"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3195,43 +3195,52 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="Y8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
@@ -3256,52 +3265,43 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="Y8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix erreures typo et push de fin de journée
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16170" windowHeight="12105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="12105"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramme de Gantt" sheetId="1" r:id="rId1"/>
@@ -790,55 +790,6 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -849,11 +800,60 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T49" sqref="T49"/>
+      <selection activeCell="AA49" sqref="AA49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1196,17 +1196,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="74"/>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="89" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74"/>
@@ -1291,7 +1291,7 @@
       <c r="R4" s="74"/>
       <c r="S4" s="74"/>
       <c r="T4" s="74"/>
-      <c r="U4" s="76" t="s">
+      <c r="U4" s="90" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="74"/>
@@ -1307,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="74"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="75" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="74"/>
@@ -1328,7 +1328,7 @@
       <c r="R5" s="74"/>
       <c r="S5" s="74"/>
       <c r="T5" s="74"/>
-      <c r="U5" s="79">
+      <c r="U5" s="76">
         <v>44319</v>
       </c>
       <c r="V5" s="74"/>
@@ -1400,187 +1400,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="82" t="s">
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="84"/>
-      <c r="Y8" s="66" t="s">
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="79"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="79"/>
+      <c r="X8" s="80"/>
+      <c r="Y8" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="67"/>
-      <c r="AA8" s="67"/>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="67"/>
-      <c r="AG8" s="67"/>
-      <c r="AH8" s="67"/>
-      <c r="AL8" s="64"/>
-      <c r="AM8" s="65"/>
-      <c r="AN8" s="65"/>
-      <c r="AO8" s="65"/>
+      <c r="Z8" s="85"/>
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="85"/>
+      <c r="AC8" s="85"/>
+      <c r="AD8" s="85"/>
+      <c r="AE8" s="85"/>
+      <c r="AF8" s="85"/>
+      <c r="AG8" s="85"/>
+      <c r="AH8" s="85"/>
+      <c r="AL8" s="82"/>
+      <c r="AM8" s="83"/>
+      <c r="AN8" s="83"/>
+      <c r="AO8" s="83"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="70" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70" t="s">
+      <c r="F9" s="72"/>
+      <c r="G9" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70" t="s">
+      <c r="H9" s="72"/>
+      <c r="I9" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="70" t="s">
+      <c r="J9" s="72"/>
+      <c r="K9" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="69"/>
-      <c r="M9" s="70" t="s">
+      <c r="L9" s="72"/>
+      <c r="M9" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="69"/>
-      <c r="O9" s="77" t="s">
+      <c r="N9" s="72"/>
+      <c r="O9" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="77" t="s">
+      <c r="P9" s="72"/>
+      <c r="Q9" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="69"/>
-      <c r="S9" s="77" t="s">
+      <c r="R9" s="72"/>
+      <c r="S9" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="69"/>
-      <c r="U9" s="77" t="s">
+      <c r="T9" s="72"/>
+      <c r="U9" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="69"/>
-      <c r="W9" s="77" t="s">
+      <c r="V9" s="72"/>
+      <c r="W9" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="69"/>
-      <c r="Y9" s="70" t="s">
+      <c r="X9" s="72"/>
+      <c r="Y9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="70" t="s">
+      <c r="Z9" s="72"/>
+      <c r="AA9" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="68" t="s">
+      <c r="AB9" s="72"/>
+      <c r="AC9" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="68" t="s">
+      <c r="AD9" s="72"/>
+      <c r="AE9" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="68" t="s">
+      <c r="AF9" s="72"/>
+      <c r="AG9" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="69"/>
+      <c r="AH9" s="72"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="70" t="s">
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="70" t="s">
+      <c r="F10" s="72"/>
+      <c r="G10" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="69"/>
-      <c r="I10" s="70" t="s">
+      <c r="H10" s="72"/>
+      <c r="I10" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70" t="s">
+      <c r="J10" s="72"/>
+      <c r="K10" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="69"/>
-      <c r="M10" s="70" t="s">
+      <c r="L10" s="72"/>
+      <c r="M10" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="69"/>
-      <c r="O10" s="77" t="s">
+      <c r="N10" s="72"/>
+      <c r="O10" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="77" t="s">
+      <c r="P10" s="72"/>
+      <c r="Q10" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="69"/>
-      <c r="S10" s="77" t="s">
+      <c r="R10" s="72"/>
+      <c r="S10" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="69"/>
-      <c r="U10" s="77" t="s">
+      <c r="T10" s="72"/>
+      <c r="U10" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="69"/>
-      <c r="W10" s="77" t="s">
+      <c r="V10" s="72"/>
+      <c r="W10" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="69"/>
-      <c r="Y10" s="70" t="s">
+      <c r="X10" s="72"/>
+      <c r="Y10" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="70" t="s">
+      <c r="Z10" s="72"/>
+      <c r="AA10" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="70" t="s">
+      <c r="AB10" s="72"/>
+      <c r="AC10" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="70" t="s">
+      <c r="AD10" s="72"/>
+      <c r="AE10" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="70" t="s">
+      <c r="AF10" s="72"/>
+      <c r="AG10" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="69"/>
+      <c r="AH10" s="72"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1634,11 +1634,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="87" t="s">
+      <c r="B12" s="64"/>
+      <c r="C12" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="88">
+      <c r="D12" s="67">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1674,9 +1674,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1710,11 +1710,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="87" t="s">
+      <c r="B14" s="70"/>
+      <c r="C14" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="88">
+      <c r="D14" s="67">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1750,9 +1750,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1786,11 +1786,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="87" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="88">
+      <c r="D16" s="67">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1826,9 +1826,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1862,11 +1862,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="87" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="88">
+      <c r="D18" s="67">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1902,9 +1902,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1938,11 +1938,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="87" t="s">
+      <c r="B20" s="64"/>
+      <c r="C20" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="88">
+      <c r="D20" s="67">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1978,9 +1978,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2014,11 +2014,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="87" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="88">
+      <c r="D22" s="67">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2054,9 +2054,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2137,11 +2137,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="87" t="s">
+      <c r="B25" s="64"/>
+      <c r="C25" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="88">
+      <c r="D25" s="67">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2177,9 +2177,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2213,11 +2213,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="87" t="s">
+      <c r="B27" s="64"/>
+      <c r="C27" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="88">
+      <c r="D27" s="67">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2253,9 +2253,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2289,11 +2289,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="87" t="s">
+      <c r="B29" s="64"/>
+      <c r="C29" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="88">
+      <c r="D29" s="67">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2329,9 +2329,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2365,11 +2365,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="87" t="s">
+      <c r="B31" s="64"/>
+      <c r="C31" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="88">
+      <c r="D31" s="67">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2405,9 +2405,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2441,11 +2441,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="87" t="s">
+      <c r="B33" s="64"/>
+      <c r="C33" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="88">
+      <c r="D33" s="67">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2480,9 +2480,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2516,11 +2516,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="87" t="s">
+      <c r="B35" s="64"/>
+      <c r="C35" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="88">
+      <c r="D35" s="67">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2555,9 +2555,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2591,11 +2591,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="87" t="s">
+      <c r="B37" s="64"/>
+      <c r="C37" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="88">
+      <c r="D37" s="67">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2630,9 +2630,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2666,11 +2666,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="87" t="s">
+      <c r="B39" s="64"/>
+      <c r="C39" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="88">
+      <c r="D39" s="67">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2705,9 +2705,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2741,11 +2741,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="87" t="s">
+      <c r="B41" s="64"/>
+      <c r="C41" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="88">
+      <c r="D41" s="67">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2781,9 +2781,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2804,7 +2804,7 @@
       <c r="V42" s="43"/>
       <c r="W42" s="42"/>
       <c r="X42" s="43"/>
-      <c r="Y42" s="39"/>
+      <c r="Y42" s="59"/>
       <c r="Z42" s="39"/>
       <c r="AA42" s="39"/>
       <c r="AB42" s="39"/>
@@ -2864,11 +2864,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="85"/>
-      <c r="C44" s="87" t="s">
+      <c r="B44" s="64"/>
+      <c r="C44" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="88">
+      <c r="D44" s="67">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2904,9 +2904,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="86"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2927,7 +2927,7 @@
       <c r="V45" s="42"/>
       <c r="W45" s="43"/>
       <c r="X45" s="42"/>
-      <c r="Y45" s="48"/>
+      <c r="Y45" s="61"/>
       <c r="Z45" s="48"/>
       <c r="AA45" s="48"/>
       <c r="AB45" s="39"/>
@@ -2940,11 +2940,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="85"/>
-      <c r="C46" s="87" t="s">
+      <c r="B46" s="64"/>
+      <c r="C46" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="88">
+      <c r="D46" s="67">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2980,9 +2980,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="86"/>
-      <c r="C47" s="86"/>
-      <c r="D47" s="86"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -3004,7 +3004,7 @@
       <c r="W47" s="43"/>
       <c r="X47" s="43"/>
       <c r="Y47" s="39"/>
-      <c r="Z47" s="39"/>
+      <c r="Z47" s="59"/>
       <c r="AA47" s="39"/>
       <c r="AB47" s="39"/>
       <c r="AC47" s="39"/>
@@ -3016,11 +3016,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="85"/>
-      <c r="C48" s="87" t="s">
+      <c r="B48" s="64"/>
+      <c r="C48" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="88">
+      <c r="D48" s="67">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3056,9 +3056,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="86"/>
-      <c r="D49" s="86"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3079,8 +3079,8 @@
       <c r="V49" s="43"/>
       <c r="W49" s="43"/>
       <c r="X49" s="43"/>
-      <c r="Y49" s="39"/>
-      <c r="Z49" s="39"/>
+      <c r="Y49" s="59"/>
+      <c r="Z49" s="59"/>
       <c r="AA49" s="39"/>
       <c r="AB49" s="39"/>
       <c r="AC49" s="39"/>
@@ -3098,16 +3098,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="90"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="81"/>
-      <c r="M50" s="90"/>
-      <c r="N50" s="81"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="68"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="68"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="69"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3118,10 +3118,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="90"/>
-      <c r="Z50" s="81"/>
-      <c r="AA50" s="90"/>
-      <c r="AB50" s="81"/>
+      <c r="Y50" s="68"/>
+      <c r="Z50" s="69"/>
+      <c r="AA50" s="68"/>
+      <c r="AB50" s="69"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3195,43 +3195,52 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="Y8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
@@ -3256,52 +3265,43 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="Y8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sécurité de l'image + doc
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -790,6 +790,55 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -800,60 +849,11 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AA49" sqref="AA49"/>
+      <selection activeCell="AA47" sqref="AA47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1196,17 +1196,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="74"/>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="75" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74"/>
@@ -1291,7 +1291,7 @@
       <c r="R4" s="74"/>
       <c r="S4" s="74"/>
       <c r="T4" s="74"/>
-      <c r="U4" s="90" t="s">
+      <c r="U4" s="76" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="74"/>
@@ -1307,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="74"/>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="78" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="74"/>
@@ -1328,7 +1328,7 @@
       <c r="R5" s="74"/>
       <c r="S5" s="74"/>
       <c r="T5" s="74"/>
-      <c r="U5" s="76">
+      <c r="U5" s="79">
         <v>44319</v>
       </c>
       <c r="V5" s="74"/>
@@ -1400,187 +1400,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="79"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="78" t="s">
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="84"/>
+      <c r="O8" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="79"/>
-      <c r="R8" s="79"/>
-      <c r="S8" s="79"/>
-      <c r="T8" s="79"/>
-      <c r="U8" s="79"/>
-      <c r="V8" s="79"/>
-      <c r="W8" s="79"/>
-      <c r="X8" s="80"/>
-      <c r="Y8" s="84" t="s">
+      <c r="P8" s="83"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="83"/>
+      <c r="S8" s="83"/>
+      <c r="T8" s="83"/>
+      <c r="U8" s="83"/>
+      <c r="V8" s="83"/>
+      <c r="W8" s="83"/>
+      <c r="X8" s="84"/>
+      <c r="Y8" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="85"/>
-      <c r="AA8" s="85"/>
-      <c r="AB8" s="85"/>
-      <c r="AC8" s="85"/>
-      <c r="AD8" s="85"/>
-      <c r="AE8" s="85"/>
-      <c r="AF8" s="85"/>
-      <c r="AG8" s="85"/>
-      <c r="AH8" s="85"/>
-      <c r="AL8" s="82"/>
-      <c r="AM8" s="83"/>
-      <c r="AN8" s="83"/>
-      <c r="AO8" s="83"/>
+      <c r="Z8" s="67"/>
+      <c r="AA8" s="67"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
+      <c r="AE8" s="67"/>
+      <c r="AF8" s="67"/>
+      <c r="AG8" s="67"/>
+      <c r="AH8" s="67"/>
+      <c r="AL8" s="64"/>
+      <c r="AM8" s="65"/>
+      <c r="AN8" s="65"/>
+      <c r="AO8" s="65"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="71" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="72"/>
-      <c r="G9" s="71" t="s">
+      <c r="F9" s="69"/>
+      <c r="G9" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="72"/>
-      <c r="I9" s="71" t="s">
+      <c r="H9" s="69"/>
+      <c r="I9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="71" t="s">
+      <c r="J9" s="69"/>
+      <c r="K9" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="72"/>
-      <c r="M9" s="71" t="s">
+      <c r="L9" s="69"/>
+      <c r="M9" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="72"/>
-      <c r="O9" s="81" t="s">
+      <c r="N9" s="69"/>
+      <c r="O9" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="81" t="s">
+      <c r="P9" s="69"/>
+      <c r="Q9" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="72"/>
-      <c r="S9" s="81" t="s">
+      <c r="R9" s="69"/>
+      <c r="S9" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="72"/>
-      <c r="U9" s="81" t="s">
+      <c r="T9" s="69"/>
+      <c r="U9" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="72"/>
-      <c r="W9" s="81" t="s">
+      <c r="V9" s="69"/>
+      <c r="W9" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="72"/>
-      <c r="Y9" s="71" t="s">
+      <c r="X9" s="69"/>
+      <c r="Y9" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="72"/>
-      <c r="AA9" s="71" t="s">
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="72"/>
-      <c r="AC9" s="86" t="s">
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="72"/>
-      <c r="AE9" s="86" t="s">
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="72"/>
-      <c r="AG9" s="86" t="s">
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="72"/>
+      <c r="AH9" s="69"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="71" t="s">
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="72"/>
-      <c r="G10" s="71" t="s">
+      <c r="F10" s="69"/>
+      <c r="G10" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="72"/>
-      <c r="I10" s="71" t="s">
+      <c r="H10" s="69"/>
+      <c r="I10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="72"/>
-      <c r="K10" s="71" t="s">
+      <c r="J10" s="69"/>
+      <c r="K10" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="72"/>
-      <c r="M10" s="71" t="s">
+      <c r="L10" s="69"/>
+      <c r="M10" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="72"/>
-      <c r="O10" s="81" t="s">
+      <c r="N10" s="69"/>
+      <c r="O10" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="81" t="s">
+      <c r="P10" s="69"/>
+      <c r="Q10" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="72"/>
-      <c r="S10" s="81" t="s">
+      <c r="R10" s="69"/>
+      <c r="S10" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="72"/>
-      <c r="U10" s="81" t="s">
+      <c r="T10" s="69"/>
+      <c r="U10" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="72"/>
-      <c r="W10" s="81" t="s">
+      <c r="V10" s="69"/>
+      <c r="W10" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="72"/>
-      <c r="Y10" s="71" t="s">
+      <c r="X10" s="69"/>
+      <c r="Y10" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="72"/>
-      <c r="AA10" s="71" t="s">
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="72"/>
-      <c r="AC10" s="71" t="s">
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="72"/>
-      <c r="AE10" s="71" t="s">
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="72"/>
-      <c r="AG10" s="71" t="s">
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="72"/>
+      <c r="AH10" s="69"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1634,11 +1634,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="66" t="s">
+      <c r="B12" s="85"/>
+      <c r="C12" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="67">
+      <c r="D12" s="88">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1674,9 +1674,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1710,11 +1710,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="66" t="s">
+      <c r="B14" s="89"/>
+      <c r="C14" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="67">
+      <c r="D14" s="88">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1750,9 +1750,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1786,11 +1786,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="66" t="s">
+      <c r="B16" s="85"/>
+      <c r="C16" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="67">
+      <c r="D16" s="88">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1826,9 +1826,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1862,11 +1862,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="66" t="s">
+      <c r="B18" s="85"/>
+      <c r="C18" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="67">
+      <c r="D18" s="88">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1902,9 +1902,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1938,11 +1938,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="66" t="s">
+      <c r="B20" s="85"/>
+      <c r="C20" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="67">
+      <c r="D20" s="88">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1978,9 +1978,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2014,11 +2014,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="66" t="s">
+      <c r="B22" s="85"/>
+      <c r="C22" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="67">
+      <c r="D22" s="88">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2054,9 +2054,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2137,11 +2137,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="66" t="s">
+      <c r="B25" s="85"/>
+      <c r="C25" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="67">
+      <c r="D25" s="88">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2177,9 +2177,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2213,11 +2213,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="66" t="s">
+      <c r="B27" s="85"/>
+      <c r="C27" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="67">
+      <c r="D27" s="88">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2253,9 +2253,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2289,11 +2289,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="66" t="s">
+      <c r="B29" s="85"/>
+      <c r="C29" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="67">
+      <c r="D29" s="88">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2329,9 +2329,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="86"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2365,11 +2365,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="66" t="s">
+      <c r="B31" s="85"/>
+      <c r="C31" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="67">
+      <c r="D31" s="88">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2405,9 +2405,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2441,11 +2441,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="66" t="s">
+      <c r="B33" s="85"/>
+      <c r="C33" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="67">
+      <c r="D33" s="88">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2480,9 +2480,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="65"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2516,11 +2516,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="66" t="s">
+      <c r="B35" s="85"/>
+      <c r="C35" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="67">
+      <c r="D35" s="88">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2555,9 +2555,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
+      <c r="B36" s="86"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2591,11 +2591,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="66" t="s">
+      <c r="B37" s="85"/>
+      <c r="C37" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="67">
+      <c r="D37" s="88">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2630,9 +2630,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2666,11 +2666,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="66" t="s">
+      <c r="B39" s="85"/>
+      <c r="C39" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="67">
+      <c r="D39" s="88">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2705,9 +2705,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2741,11 +2741,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="66" t="s">
+      <c r="B41" s="85"/>
+      <c r="C41" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="67">
+      <c r="D41" s="88">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2781,9 +2781,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2806,7 +2806,7 @@
       <c r="X42" s="43"/>
       <c r="Y42" s="59"/>
       <c r="Z42" s="39"/>
-      <c r="AA42" s="39"/>
+      <c r="AA42" s="37"/>
       <c r="AB42" s="39"/>
       <c r="AC42" s="48"/>
       <c r="AD42" s="48"/>
@@ -2864,11 +2864,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="66" t="s">
+      <c r="B44" s="85"/>
+      <c r="C44" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="67">
+      <c r="D44" s="88">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2904,9 +2904,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2929,7 +2929,7 @@
       <c r="X45" s="42"/>
       <c r="Y45" s="61"/>
       <c r="Z45" s="48"/>
-      <c r="AA45" s="48"/>
+      <c r="AA45" s="61"/>
       <c r="AB45" s="39"/>
       <c r="AC45" s="48"/>
       <c r="AD45" s="48"/>
@@ -2940,11 +2940,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="66" t="s">
+      <c r="B46" s="85"/>
+      <c r="C46" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="67">
+      <c r="D46" s="88">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2980,9 +2980,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="65"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="65"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -3016,11 +3016,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="66" t="s">
+      <c r="B48" s="85"/>
+      <c r="C48" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="67">
+      <c r="D48" s="88">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3056,9 +3056,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="65"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="86"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3081,7 +3081,7 @@
       <c r="X49" s="43"/>
       <c r="Y49" s="59"/>
       <c r="Z49" s="59"/>
-      <c r="AA49" s="39"/>
+      <c r="AA49" s="59"/>
       <c r="AB49" s="39"/>
       <c r="AC49" s="39"/>
       <c r="AD49" s="39"/>
@@ -3098,16 +3098,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="68"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="68"/>
-      <c r="J50" s="69"/>
-      <c r="K50" s="68"/>
-      <c r="L50" s="69"/>
-      <c r="M50" s="68"/>
-      <c r="N50" s="69"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="81"/>
+      <c r="I50" s="90"/>
+      <c r="J50" s="81"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="81"/>
+      <c r="M50" s="90"/>
+      <c r="N50" s="81"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3118,10 +3118,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="68"/>
-      <c r="Z50" s="69"/>
-      <c r="AA50" s="68"/>
-      <c r="AB50" s="69"/>
+      <c r="Y50" s="90"/>
+      <c r="Z50" s="81"/>
+      <c r="AA50" s="90"/>
+      <c r="AB50" s="81"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3195,6 +3195,89 @@
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="AL8:AO8"/>
     <mergeCell ref="Y8:AH8"/>
     <mergeCell ref="AC9:AD9"/>
@@ -3219,89 +3302,6 @@
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
entêtes, doc et suppression des examples tcpdf
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -790,55 +790,6 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -849,11 +800,60 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,8 +1147,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AA47" sqref="AA47"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC49" sqref="AC49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1196,17 +1196,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="74"/>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="89" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74"/>
@@ -1291,7 +1291,7 @@
       <c r="R4" s="74"/>
       <c r="S4" s="74"/>
       <c r="T4" s="74"/>
-      <c r="U4" s="76" t="s">
+      <c r="U4" s="90" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="74"/>
@@ -1307,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="74"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="75" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="74"/>
@@ -1328,7 +1328,7 @@
       <c r="R5" s="74"/>
       <c r="S5" s="74"/>
       <c r="T5" s="74"/>
-      <c r="U5" s="79">
+      <c r="U5" s="76">
         <v>44319</v>
       </c>
       <c r="V5" s="74"/>
@@ -1400,187 +1400,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="82" t="s">
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="84"/>
-      <c r="Y8" s="66" t="s">
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="79"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="79"/>
+      <c r="X8" s="80"/>
+      <c r="Y8" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="67"/>
-      <c r="AA8" s="67"/>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="67"/>
-      <c r="AG8" s="67"/>
-      <c r="AH8" s="67"/>
-      <c r="AL8" s="64"/>
-      <c r="AM8" s="65"/>
-      <c r="AN8" s="65"/>
-      <c r="AO8" s="65"/>
+      <c r="Z8" s="85"/>
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="85"/>
+      <c r="AC8" s="85"/>
+      <c r="AD8" s="85"/>
+      <c r="AE8" s="85"/>
+      <c r="AF8" s="85"/>
+      <c r="AG8" s="85"/>
+      <c r="AH8" s="85"/>
+      <c r="AL8" s="82"/>
+      <c r="AM8" s="83"/>
+      <c r="AN8" s="83"/>
+      <c r="AO8" s="83"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="70" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70" t="s">
+      <c r="F9" s="72"/>
+      <c r="G9" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70" t="s">
+      <c r="H9" s="72"/>
+      <c r="I9" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="70" t="s">
+      <c r="J9" s="72"/>
+      <c r="K9" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="69"/>
-      <c r="M9" s="70" t="s">
+      <c r="L9" s="72"/>
+      <c r="M9" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="69"/>
-      <c r="O9" s="77" t="s">
+      <c r="N9" s="72"/>
+      <c r="O9" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="77" t="s">
+      <c r="P9" s="72"/>
+      <c r="Q9" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="69"/>
-      <c r="S9" s="77" t="s">
+      <c r="R9" s="72"/>
+      <c r="S9" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="69"/>
-      <c r="U9" s="77" t="s">
+      <c r="T9" s="72"/>
+      <c r="U9" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="69"/>
-      <c r="W9" s="77" t="s">
+      <c r="V9" s="72"/>
+      <c r="W9" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="69"/>
-      <c r="Y9" s="70" t="s">
+      <c r="X9" s="72"/>
+      <c r="Y9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="70" t="s">
+      <c r="Z9" s="72"/>
+      <c r="AA9" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="68" t="s">
+      <c r="AB9" s="72"/>
+      <c r="AC9" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="68" t="s">
+      <c r="AD9" s="72"/>
+      <c r="AE9" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="68" t="s">
+      <c r="AF9" s="72"/>
+      <c r="AG9" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="69"/>
+      <c r="AH9" s="72"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="70" t="s">
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="70" t="s">
+      <c r="F10" s="72"/>
+      <c r="G10" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="69"/>
-      <c r="I10" s="70" t="s">
+      <c r="H10" s="72"/>
+      <c r="I10" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70" t="s">
+      <c r="J10" s="72"/>
+      <c r="K10" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="69"/>
-      <c r="M10" s="70" t="s">
+      <c r="L10" s="72"/>
+      <c r="M10" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="69"/>
-      <c r="O10" s="77" t="s">
+      <c r="N10" s="72"/>
+      <c r="O10" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="77" t="s">
+      <c r="P10" s="72"/>
+      <c r="Q10" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="69"/>
-      <c r="S10" s="77" t="s">
+      <c r="R10" s="72"/>
+      <c r="S10" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="69"/>
-      <c r="U10" s="77" t="s">
+      <c r="T10" s="72"/>
+      <c r="U10" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="69"/>
-      <c r="W10" s="77" t="s">
+      <c r="V10" s="72"/>
+      <c r="W10" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="69"/>
-      <c r="Y10" s="70" t="s">
+      <c r="X10" s="72"/>
+      <c r="Y10" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="70" t="s">
+      <c r="Z10" s="72"/>
+      <c r="AA10" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="70" t="s">
+      <c r="AB10" s="72"/>
+      <c r="AC10" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="70" t="s">
+      <c r="AD10" s="72"/>
+      <c r="AE10" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="70" t="s">
+      <c r="AF10" s="72"/>
+      <c r="AG10" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="69"/>
+      <c r="AH10" s="72"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1634,11 +1634,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="87" t="s">
+      <c r="B12" s="64"/>
+      <c r="C12" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="88">
+      <c r="D12" s="67">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1674,9 +1674,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1710,11 +1710,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="87" t="s">
+      <c r="B14" s="70"/>
+      <c r="C14" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="88">
+      <c r="D14" s="67">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1750,9 +1750,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1786,11 +1786,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="87" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="88">
+      <c r="D16" s="67">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1826,9 +1826,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1862,11 +1862,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="87" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="88">
+      <c r="D18" s="67">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1902,9 +1902,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1938,11 +1938,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="87" t="s">
+      <c r="B20" s="64"/>
+      <c r="C20" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="88">
+      <c r="D20" s="67">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1978,9 +1978,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2014,11 +2014,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="87" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="88">
+      <c r="D22" s="67">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2054,9 +2054,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2137,11 +2137,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="87" t="s">
+      <c r="B25" s="64"/>
+      <c r="C25" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="88">
+      <c r="D25" s="67">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2177,9 +2177,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2213,11 +2213,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="87" t="s">
+      <c r="B27" s="64"/>
+      <c r="C27" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="88">
+      <c r="D27" s="67">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2253,9 +2253,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2289,11 +2289,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="87" t="s">
+      <c r="B29" s="64"/>
+      <c r="C29" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="88">
+      <c r="D29" s="67">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2329,9 +2329,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2365,11 +2365,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="87" t="s">
+      <c r="B31" s="64"/>
+      <c r="C31" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="88">
+      <c r="D31" s="67">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2405,9 +2405,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2441,11 +2441,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="87" t="s">
+      <c r="B33" s="64"/>
+      <c r="C33" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="88">
+      <c r="D33" s="67">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2480,9 +2480,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2516,11 +2516,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="87" t="s">
+      <c r="B35" s="64"/>
+      <c r="C35" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="88">
+      <c r="D35" s="67">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2555,9 +2555,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2591,11 +2591,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="87" t="s">
+      <c r="B37" s="64"/>
+      <c r="C37" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="88">
+      <c r="D37" s="67">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2630,9 +2630,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2666,11 +2666,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="87" t="s">
+      <c r="B39" s="64"/>
+      <c r="C39" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="88">
+      <c r="D39" s="67">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2705,9 +2705,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2741,11 +2741,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="87" t="s">
+      <c r="B41" s="64"/>
+      <c r="C41" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="88">
+      <c r="D41" s="67">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2781,9 +2781,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2864,11 +2864,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="85"/>
-      <c r="C44" s="87" t="s">
+      <c r="B44" s="64"/>
+      <c r="C44" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="88">
+      <c r="D44" s="67">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2904,9 +2904,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="86"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2940,11 +2940,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="85"/>
-      <c r="C46" s="87" t="s">
+      <c r="B46" s="64"/>
+      <c r="C46" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="88">
+      <c r="D46" s="67">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2980,9 +2980,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="86"/>
-      <c r="C47" s="86"/>
-      <c r="D47" s="86"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -3005,8 +3005,8 @@
       <c r="X47" s="43"/>
       <c r="Y47" s="39"/>
       <c r="Z47" s="59"/>
-      <c r="AA47" s="39"/>
-      <c r="AB47" s="39"/>
+      <c r="AA47" s="59"/>
+      <c r="AB47" s="59"/>
       <c r="AC47" s="39"/>
       <c r="AD47" s="39"/>
       <c r="AE47" s="39"/>
@@ -3016,11 +3016,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="85"/>
-      <c r="C48" s="87" t="s">
+      <c r="B48" s="64"/>
+      <c r="C48" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="88">
+      <c r="D48" s="67">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3056,9 +3056,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="86"/>
-      <c r="D49" s="86"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3082,7 +3082,7 @@
       <c r="Y49" s="59"/>
       <c r="Z49" s="59"/>
       <c r="AA49" s="59"/>
-      <c r="AB49" s="39"/>
+      <c r="AB49" s="59"/>
       <c r="AC49" s="39"/>
       <c r="AD49" s="39"/>
       <c r="AE49" s="39"/>
@@ -3098,16 +3098,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="90"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="81"/>
-      <c r="M50" s="90"/>
-      <c r="N50" s="81"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="68"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="68"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="69"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3118,10 +3118,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="90"/>
-      <c r="Z50" s="81"/>
-      <c r="AA50" s="90"/>
-      <c r="AB50" s="81"/>
+      <c r="Y50" s="68"/>
+      <c r="Z50" s="69"/>
+      <c r="AA50" s="68"/>
+      <c r="AB50" s="69"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3195,43 +3195,52 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="Y8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
@@ -3256,52 +3265,43 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="Y8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
push de fin de journée
</commit_message>
<xml_diff>
--- a/doc/2021TPI_BG_Plannification_Reel.xlsx
+++ b/doc/2021TPI_BG_Plannification_Reel.xlsx
@@ -790,55 +790,6 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -849,11 +800,60 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD47" sqref="AD47"/>
+      <selection activeCell="AD49" sqref="AD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1196,17 +1196,17 @@
     </row>
     <row r="2" spans="1:41" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
       <c r="K2" s="9"/>
       <c r="L2" s="49"/>
       <c r="M2" s="52"/>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="74"/>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="89" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74"/>
@@ -1291,7 +1291,7 @@
       <c r="R4" s="74"/>
       <c r="S4" s="74"/>
       <c r="T4" s="74"/>
-      <c r="U4" s="76" t="s">
+      <c r="U4" s="90" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="74"/>
@@ -1307,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="74"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="75" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="74"/>
@@ -1328,7 +1328,7 @@
       <c r="R5" s="74"/>
       <c r="S5" s="74"/>
       <c r="T5" s="74"/>
-      <c r="U5" s="79">
+      <c r="U5" s="76">
         <v>44319</v>
       </c>
       <c r="V5" s="74"/>
@@ -1400,187 +1400,187 @@
     </row>
     <row r="8" spans="1:41" ht="17.25" customHeight="1">
       <c r="A8" s="20"/>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="82" t="s">
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="84"/>
-      <c r="Y8" s="66" t="s">
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="79"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="79"/>
+      <c r="X8" s="80"/>
+      <c r="Y8" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="67"/>
-      <c r="AA8" s="67"/>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="67"/>
-      <c r="AG8" s="67"/>
-      <c r="AH8" s="67"/>
-      <c r="AL8" s="64"/>
-      <c r="AM8" s="65"/>
-      <c r="AN8" s="65"/>
-      <c r="AO8" s="65"/>
+      <c r="Z8" s="85"/>
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="85"/>
+      <c r="AC8" s="85"/>
+      <c r="AD8" s="85"/>
+      <c r="AE8" s="85"/>
+      <c r="AF8" s="85"/>
+      <c r="AG8" s="85"/>
+      <c r="AH8" s="85"/>
+      <c r="AL8" s="82"/>
+      <c r="AM8" s="83"/>
+      <c r="AN8" s="83"/>
+      <c r="AO8" s="83"/>
     </row>
     <row r="9" spans="1:41" ht="17.25" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="70" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70" t="s">
+      <c r="F9" s="72"/>
+      <c r="G9" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70" t="s">
+      <c r="H9" s="72"/>
+      <c r="I9" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="70" t="s">
+      <c r="J9" s="72"/>
+      <c r="K9" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="69"/>
-      <c r="M9" s="70" t="s">
+      <c r="L9" s="72"/>
+      <c r="M9" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="69"/>
-      <c r="O9" s="77" t="s">
+      <c r="N9" s="72"/>
+      <c r="O9" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="77" t="s">
+      <c r="P9" s="72"/>
+      <c r="Q9" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="69"/>
-      <c r="S9" s="77" t="s">
+      <c r="R9" s="72"/>
+      <c r="S9" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="69"/>
-      <c r="U9" s="77" t="s">
+      <c r="T9" s="72"/>
+      <c r="U9" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="69"/>
-      <c r="W9" s="77" t="s">
+      <c r="V9" s="72"/>
+      <c r="W9" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="X9" s="69"/>
-      <c r="Y9" s="70" t="s">
+      <c r="X9" s="72"/>
+      <c r="Y9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="70" t="s">
+      <c r="Z9" s="72"/>
+      <c r="AA9" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="68" t="s">
+      <c r="AB9" s="72"/>
+      <c r="AC9" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="68" t="s">
+      <c r="AD9" s="72"/>
+      <c r="AE9" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="68" t="s">
+      <c r="AF9" s="72"/>
+      <c r="AG9" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="AH9" s="69"/>
+      <c r="AH9" s="72"/>
     </row>
     <row r="10" spans="1:41" ht="17.25" customHeight="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="70" t="s">
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="70" t="s">
+      <c r="F10" s="72"/>
+      <c r="G10" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="69"/>
-      <c r="I10" s="70" t="s">
+      <c r="H10" s="72"/>
+      <c r="I10" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70" t="s">
+      <c r="J10" s="72"/>
+      <c r="K10" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="69"/>
-      <c r="M10" s="70" t="s">
+      <c r="L10" s="72"/>
+      <c r="M10" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="69"/>
-      <c r="O10" s="77" t="s">
+      <c r="N10" s="72"/>
+      <c r="O10" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="77" t="s">
+      <c r="P10" s="72"/>
+      <c r="Q10" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="69"/>
-      <c r="S10" s="77" t="s">
+      <c r="R10" s="72"/>
+      <c r="S10" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="69"/>
-      <c r="U10" s="77" t="s">
+      <c r="T10" s="72"/>
+      <c r="U10" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="69"/>
-      <c r="W10" s="77" t="s">
+      <c r="V10" s="72"/>
+      <c r="W10" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="X10" s="69"/>
-      <c r="Y10" s="70" t="s">
+      <c r="X10" s="72"/>
+      <c r="Y10" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="70" t="s">
+      <c r="Z10" s="72"/>
+      <c r="AA10" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="70" t="s">
+      <c r="AB10" s="72"/>
+      <c r="AC10" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="70" t="s">
+      <c r="AD10" s="72"/>
+      <c r="AE10" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="70" t="s">
+      <c r="AF10" s="72"/>
+      <c r="AG10" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="AH10" s="69"/>
+      <c r="AH10" s="72"/>
       <c r="AI10" s="50" t="s">
         <v>24</v>
       </c>
@@ -1634,11 +1634,11 @@
     </row>
     <row r="12" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="87" t="s">
+      <c r="B12" s="64"/>
+      <c r="C12" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="88">
+      <c r="D12" s="67">
         <v>1</v>
       </c>
       <c r="E12" s="35"/>
@@ -1674,9 +1674,9 @@
     </row>
     <row r="13" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="59"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
@@ -1710,11 +1710,11 @@
     </row>
     <row r="14" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="87" t="s">
+      <c r="B14" s="70"/>
+      <c r="C14" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="88">
+      <c r="D14" s="67">
         <v>2</v>
       </c>
       <c r="E14" s="40"/>
@@ -1750,9 +1750,9 @@
     </row>
     <row r="15" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
       <c r="G15" s="36"/>
@@ -1786,11 +1786,11 @@
     </row>
     <row r="16" spans="1:41" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="87" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="88">
+      <c r="D16" s="67">
         <v>2</v>
       </c>
       <c r="E16" s="37"/>
@@ -1826,9 +1826,9 @@
     </row>
     <row r="17" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A17" s="30"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="59"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -1862,11 +1862,11 @@
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A18" s="30"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="87" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="88">
+      <c r="D18" s="67">
         <v>2</v>
       </c>
       <c r="E18" s="36"/>
@@ -1902,9 +1902,9 @@
     </row>
     <row r="19" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A19" s="30"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="37"/>
       <c r="F19" s="59"/>
       <c r="G19" s="36"/>
@@ -1938,11 +1938,11 @@
     </row>
     <row r="20" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A20" s="30"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="87" t="s">
+      <c r="B20" s="64"/>
+      <c r="C20" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="88">
+      <c r="D20" s="67">
         <v>1</v>
       </c>
       <c r="E20" s="57"/>
@@ -1978,9 +1978,9 @@
     </row>
     <row r="21" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A21" s="30"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="60"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -2014,11 +2014,11 @@
     </row>
     <row r="22" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A22" s="30"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="87" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="88">
+      <c r="D22" s="67">
         <v>2</v>
       </c>
       <c r="E22" s="53"/>
@@ -2054,9 +2054,9 @@
     </row>
     <row r="23" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="36"/>
       <c r="F23" s="59"/>
       <c r="G23" s="36"/>
@@ -2137,11 +2137,11 @@
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A25" s="30"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="87" t="s">
+      <c r="B25" s="64"/>
+      <c r="C25" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="88">
+      <c r="D25" s="67">
         <v>4</v>
       </c>
       <c r="E25" s="37"/>
@@ -2177,9 +2177,9 @@
     </row>
     <row r="26" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A26" s="30"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
       <c r="E26" s="41"/>
       <c r="F26" s="36"/>
       <c r="G26" s="59"/>
@@ -2213,11 +2213,11 @@
     </row>
     <row r="27" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="30"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="87" t="s">
+      <c r="B27" s="64"/>
+      <c r="C27" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="88">
+      <c r="D27" s="67">
         <v>6</v>
       </c>
       <c r="E27" s="41"/>
@@ -2253,9 +2253,9 @@
     </row>
     <row r="28" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="30"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="41"/>
       <c r="F28" s="36"/>
       <c r="G28" s="37"/>
@@ -2289,11 +2289,11 @@
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="30"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="87" t="s">
+      <c r="B29" s="64"/>
+      <c r="C29" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="88">
+      <c r="D29" s="67">
         <v>2</v>
       </c>
       <c r="E29" s="41"/>
@@ -2329,9 +2329,9 @@
     </row>
     <row r="30" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="30"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="41"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -2365,11 +2365,11 @@
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="30"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="87" t="s">
+      <c r="B31" s="64"/>
+      <c r="C31" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="88">
+      <c r="D31" s="67">
         <v>2</v>
       </c>
       <c r="E31" s="41"/>
@@ -2405,9 +2405,9 @@
     </row>
     <row r="32" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="41"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
@@ -2441,11 +2441,11 @@
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A33" s="30"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="87" t="s">
+      <c r="B33" s="64"/>
+      <c r="C33" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="88">
+      <c r="D33" s="67">
         <v>3</v>
       </c>
       <c r="E33" s="41"/>
@@ -2480,9 +2480,9 @@
     </row>
     <row r="34" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A34" s="30"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
       <c r="E34" s="41"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
@@ -2516,11 +2516,11 @@
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A35" s="30"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="87" t="s">
+      <c r="B35" s="64"/>
+      <c r="C35" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="88">
+      <c r="D35" s="67">
         <v>4</v>
       </c>
       <c r="E35" s="41"/>
@@ -2555,9 +2555,9 @@
     </row>
     <row r="36" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A36" s="30"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
       <c r="E36" s="41"/>
       <c r="F36" s="36"/>
       <c r="G36" s="60"/>
@@ -2591,11 +2591,11 @@
     </row>
     <row r="37" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="30"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="87" t="s">
+      <c r="B37" s="64"/>
+      <c r="C37" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="88">
+      <c r="D37" s="67">
         <v>4</v>
       </c>
       <c r="E37" s="41"/>
@@ -2630,9 +2630,9 @@
     </row>
     <row r="38" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A38" s="30"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
       <c r="E38" s="41"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
@@ -2666,11 +2666,11 @@
     </row>
     <row r="39" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A39" s="30"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="87" t="s">
+      <c r="B39" s="64"/>
+      <c r="C39" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="88">
+      <c r="D39" s="67">
         <v>6</v>
       </c>
       <c r="E39" s="41"/>
@@ -2705,9 +2705,9 @@
     </row>
     <row r="40" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A40" s="30"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="41"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -2741,11 +2741,11 @@
     </row>
     <row r="41" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A41" s="30"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="87" t="s">
+      <c r="B41" s="64"/>
+      <c r="C41" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="88">
+      <c r="D41" s="67">
         <v>10</v>
       </c>
       <c r="E41" s="41"/>
@@ -2781,9 +2781,9 @@
     </row>
     <row r="42" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A42" s="30"/>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="41"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -2864,11 +2864,11 @@
     </row>
     <row r="44" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A44" s="30"/>
-      <c r="B44" s="85"/>
-      <c r="C44" s="87" t="s">
+      <c r="B44" s="64"/>
+      <c r="C44" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="88">
+      <c r="D44" s="67">
         <v>8</v>
       </c>
       <c r="E44" s="39"/>
@@ -2904,9 +2904,9 @@
     </row>
     <row r="45" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A45" s="30"/>
-      <c r="B45" s="86"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
       <c r="E45" s="47"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
@@ -2932,7 +2932,7 @@
       <c r="AA45" s="61"/>
       <c r="AB45" s="39"/>
       <c r="AC45" s="48"/>
-      <c r="AD45" s="48"/>
+      <c r="AD45" s="61"/>
       <c r="AE45" s="48"/>
       <c r="AF45" s="48"/>
       <c r="AG45" s="48"/>
@@ -2940,11 +2940,11 @@
     </row>
     <row r="46" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A46" s="30"/>
-      <c r="B46" s="85"/>
-      <c r="C46" s="87" t="s">
+      <c r="B46" s="64"/>
+      <c r="C46" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="88">
+      <c r="D46" s="67">
         <v>24</v>
       </c>
       <c r="E46" s="47"/>
@@ -2980,9 +2980,9 @@
     </row>
     <row r="47" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="86"/>
-      <c r="C47" s="86"/>
-      <c r="D47" s="86"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
       <c r="E47" s="59"/>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -3008,7 +3008,7 @@
       <c r="AA47" s="59"/>
       <c r="AB47" s="59"/>
       <c r="AC47" s="59"/>
-      <c r="AD47" s="39"/>
+      <c r="AD47" s="59"/>
       <c r="AE47" s="39"/>
       <c r="AF47" s="39"/>
       <c r="AG47" s="48"/>
@@ -3016,11 +3016,11 @@
     </row>
     <row r="48" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A48" s="30"/>
-      <c r="B48" s="85"/>
-      <c r="C48" s="87" t="s">
+      <c r="B48" s="64"/>
+      <c r="C48" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="88">
+      <c r="D48" s="67">
         <v>5</v>
       </c>
       <c r="E48" s="46"/>
@@ -3056,9 +3056,9 @@
     </row>
     <row r="49" spans="1:35" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A49" s="30"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="86"/>
-      <c r="D49" s="86"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3084,7 +3084,7 @@
       <c r="AA49" s="59"/>
       <c r="AB49" s="59"/>
       <c r="AC49" s="59"/>
-      <c r="AD49" s="39"/>
+      <c r="AD49" s="59"/>
       <c r="AE49" s="39"/>
       <c r="AF49" s="39"/>
       <c r="AG49" s="48"/>
@@ -3098,16 +3098,16 @@
         <f>SUM(D11,D24,D43)</f>
         <v>88</v>
       </c>
-      <c r="E50" s="90"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="81"/>
-      <c r="M50" s="90"/>
-      <c r="N50" s="81"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="68"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="68"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="69"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -3118,10 +3118,10 @@
       <c r="V50" s="33"/>
       <c r="W50" s="33"/>
       <c r="X50" s="33"/>
-      <c r="Y50" s="90"/>
-      <c r="Z50" s="81"/>
-      <c r="AA50" s="90"/>
-      <c r="AB50" s="81"/>
+      <c r="Y50" s="68"/>
+      <c r="Z50" s="69"/>
+      <c r="AA50" s="68"/>
+      <c r="AB50" s="69"/>
       <c r="AC50" s="50"/>
       <c r="AD50" s="50"/>
       <c r="AE50" s="50"/>
@@ -3195,43 +3195,52 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="Y8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:T5"/>
+    <mergeCell ref="U5:AA5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:N8"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
@@ -3256,52 +3265,43 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:T5"/>
-    <mergeCell ref="U5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:N8"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="Y8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Y50:Z50"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>